<commit_message>
go shared table full
</commit_message>
<xml_diff>
--- a/Output/SuppTables/Shared_GO.xlsx
+++ b/Output/SuppTables/Shared_GO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jillashey/Desktop/PutnamLab/Repositories/SedimentStress/SedimentStress/Output/SuppTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DBB9CFDC-4880-D047-A7E5-66DAFA68DD65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F704D710-C99F-CB4D-9756-6F2F207D4EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6980" yWindow="2000" windowWidth="28860" windowHeight="17780" xr2:uid="{463EAF44-39AF-B74B-A9CF-96AD4C6642C9}"/>
+    <workbookView xWindow="16520" yWindow="500" windowWidth="19320" windowHeight="20740" xr2:uid="{463EAF44-39AF-B74B-A9CF-96AD4C6642C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Full" sheetId="17" r:id="rId1"/>
@@ -28,7 +28,6 @@
     <sheet name="Ofav+Pacuta" sheetId="14" r:id="rId13"/>
     <sheet name="Mcap+Pacuta" sheetId="13" r:id="rId14"/>
     <sheet name="Pacuta+Plob" sheetId="15" r:id="rId15"/>
-    <sheet name="Sheet16" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -50,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="120">
   <si>
     <t>A.cervicornis + M.cavernosa + M.capitata</t>
   </si>
@@ -181,102 +180,9 @@
     <t>Mcap + Pacuta (20)</t>
   </si>
   <si>
-    <t>GO:0038166 - angiotensin-activated signaling pathway, NO GO SLIM </t>
-  </si>
-  <si>
-    <t>GO:0009785 - ​​blue light signaling pathway, signal transduction </t>
-  </si>
-  <si>
-    <t>GO:0015670 - carbon dioxide transport, transport </t>
-  </si>
-  <si>
-    <t>GO:0071300 - cellular response to retinoic acid, NO GO SLIM</t>
-  </si>
-  <si>
-    <t>GO:0035116 - embryonic hindlimb morphogenesis, developmental processes </t>
-  </si>
-  <si>
-    <t>GO:0007157 - heterophilic cell adhesion, cell adhesion </t>
-  </si>
-  <si>
-    <t>GO:0045780 - positive regulation of bone resorption, other biological processes  </t>
-  </si>
-  <si>
-    <t>GO:0032849 - positive regulation of cellular pH reduction, other biological processes  </t>
-  </si>
-  <si>
-    <t>GO:2001150 - positive regulation of dipeptide transmembrane transport, NO GO SLIM</t>
-  </si>
-  <si>
-    <t>GO:0035794 - positive regulation of mitochondrial membrane permeability, NO GO SLIM</t>
-  </si>
-  <si>
-    <t>GO:0045672 - positive regulation of osteoclast differentiation, developmental processes</t>
-  </si>
-  <si>
-    <t>GO:0051091 - positive regulation of transcription factor activity, RNA metabolism </t>
-  </si>
-  <si>
-    <t>GO:2000850 - negative regulation of glucocorticoid secretion, NO GO SLIM </t>
-  </si>
-  <si>
-    <t>GO:0055114 - oxidation reduction, other biological processes </t>
-  </si>
-  <si>
-    <t>GO:2001225 - regulation of chloride transport, NO GO SLIM</t>
-  </si>
-  <si>
-    <t>GO:0014823 - response to activity, other biological processes </t>
-  </si>
-  <si>
-    <t>GO:0033762 - response to glucagon stimulus, other biological processes  </t>
-  </si>
-  <si>
-    <t>GO:0048265 - response to pain, stress response  </t>
-  </si>
-  <si>
-    <t>GO:0009268 - response to pH, other biological processes  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0046903 - secretion, transport  </t>
-  </si>
-  <si>
     <t>Pacuta + Plob (11)</t>
   </si>
   <si>
-    <t>GO:0044335 - canonical Wnt signaling pathway involved in neural crest cell differentiation, NO GO SLIM </t>
-  </si>
-  <si>
-    <t>GO:0071476 - cellular hypotonic response, NO GO SLIM </t>
-  </si>
-  <si>
-    <t>GO:0000578 - embryonic axis specification, developmental processes  </t>
-  </si>
-  <si>
-    <t>GO:0048568 - embryonic organ development, developmental processes </t>
-  </si>
-  <si>
-    <t>GO:0003197 - endocardial cushion development, NO GO SLIM </t>
-  </si>
-  <si>
-    <t>GO:0001654 - eye development, developmental processes  </t>
-  </si>
-  <si>
-    <t>GO:2000044 - negative regulation of cardiac cell fate specification, NO GO SLIM </t>
-  </si>
-  <si>
-    <t>GO:0014036 - neural crest cell fate specification, developmental processes &amp; cell organization and biogenesis</t>
-  </si>
-  <si>
-    <t>GO:0021999 - neural plate anterior/posterior regionalization, developmental processes  </t>
-  </si>
-  <si>
-    <t>GO:0042752 - regulation of circadian rhythm, other biological processes </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0060061 - Spemann organizer formation, cell-cell signaling  </t>
-  </si>
-  <si>
     <t>other biological processes</t>
   </si>
   <si>
@@ -347,6 +253,162 @@
   </si>
   <si>
     <t>​​response to stimulus (GO:0050896)</t>
+  </si>
+  <si>
+    <t>​​blue light signaling pathway (GO:0009785)</t>
+  </si>
+  <si>
+    <t>signal transduction </t>
+  </si>
+  <si>
+    <t>developmental processes </t>
+  </si>
+  <si>
+    <t>embryonic hindlimb morphogenesis (GO:0035116)</t>
+  </si>
+  <si>
+    <t>positive regulation of osteoclast differentiation (GO:0045672)</t>
+  </si>
+  <si>
+    <t>cell adhesion </t>
+  </si>
+  <si>
+    <t>heterophilic cell adhesion (GO:0007157)</t>
+  </si>
+  <si>
+    <t>other biological processes  </t>
+  </si>
+  <si>
+    <t>positive regulation of bone resorption (GO:0045780)</t>
+  </si>
+  <si>
+    <t>positive regulation of cellular pH reduction (GO:0032849)</t>
+  </si>
+  <si>
+    <t>oxidation reduction (GO:0055114)</t>
+  </si>
+  <si>
+    <t>response to activity (GO:0014823)</t>
+  </si>
+  <si>
+    <t>response to glucagon stimulus (GO:0033762)</t>
+  </si>
+  <si>
+    <t>response to pH (GO:0009268)</t>
+  </si>
+  <si>
+    <t>positive regulation of transcription factor activity (GO:0051091)</t>
+  </si>
+  <si>
+    <t>stress response  </t>
+  </si>
+  <si>
+    <t>response to pain (GO:0048265)</t>
+  </si>
+  <si>
+    <t>transport </t>
+  </si>
+  <si>
+    <t>carbon dioxide transport (GO:0015670)</t>
+  </si>
+  <si>
+    <t>secretion (GO:0046903)</t>
+  </si>
+  <si>
+    <t>NO GO SLIM </t>
+  </si>
+  <si>
+    <t>angiotensin-activated signaling pathway (GO:0038166)</t>
+  </si>
+  <si>
+    <t>cellular response to retinoic acid (GO:0071300)</t>
+  </si>
+  <si>
+    <t>positive regulation of dipeptide transmembrane transport (GO:2001150)</t>
+  </si>
+  <si>
+    <t>positive regulation of mitochondrial membrane permeability (GO:0035794)</t>
+  </si>
+  <si>
+    <t>negative regulation of glucocorticoid secretion (GO:2000850)</t>
+  </si>
+  <si>
+    <t>regulation of chloride transport (GO:2001225)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cell-cell signaling  </t>
+  </si>
+  <si>
+    <t>Spemann organizer formation (GO:0060061)</t>
+  </si>
+  <si>
+    <t>neural crest cell fate specification (GO:0014036)</t>
+  </si>
+  <si>
+    <t>developmental processes  </t>
+  </si>
+  <si>
+    <t>embryonic axis specification (GO:0000578)</t>
+  </si>
+  <si>
+    <t>embryonic organ development (GO:0048568)</t>
+  </si>
+  <si>
+    <t>eye development (GO:0001654)</t>
+  </si>
+  <si>
+    <t>neural plate anterior/posterior regionalization (GO:0021999)</t>
+  </si>
+  <si>
+    <t>other biological processes </t>
+  </si>
+  <si>
+    <t>regulation of circadian rhythm (GO:0042752)</t>
+  </si>
+  <si>
+    <t>canonical Wnt signaling pathway involved in neural crest cell differentiation (GO:0044335)</t>
+  </si>
+  <si>
+    <t>cellular hypotonic response (GO:0071476)</t>
+  </si>
+  <si>
+    <t>endocardial cushion development (GO:0003197)</t>
+  </si>
+  <si>
+    <t>negative regulation of cardiac cell fate specification (GO:2000044)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Averv + Ofav </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acerv + Mcap </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acerv + Pacuta </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acerv + Plob </t>
+  </si>
+  <si>
+    <t>Mcap + Pacuta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pacuta + Plob </t>
+  </si>
+  <si>
+    <t>maintenance of gastrointestinal epithelium (GO:0030277)</t>
+  </si>
+  <si>
+    <t>Wnt receptor signaling pathway (GO:0016055)</t>
+  </si>
+  <si>
+    <t>Mo-molybdopterin cofactor biosynthetic process (GO:0006777)</t>
+  </si>
+  <si>
+    <t>cellular response to starvation (GO:0009267)</t>
+  </si>
+  <si>
+    <t>mesenchymal stem cell maintenance involved in nephron morphogenesis (GO:0072038)</t>
   </si>
 </sst>
 </file>
@@ -499,7 +561,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -526,6 +588,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -566,24 +630,9 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -593,9 +642,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -630,6 +676,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -946,385 +1016,536 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{113029E7-F384-C24D-A58A-6D6AAA957483}">
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" zoomScale="56" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41" style="43" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.83203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="84.5" style="44" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.5" style="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35" style="39" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="112" style="40" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="10.83203125" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="23" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:3" s="25" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="27" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="47" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="50" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="47" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="34" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+    <row r="5" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="50" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="34" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
-      <c r="B6" s="33" t="s">
+    <row r="6" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="32"/>
+      <c r="B6" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="50" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="34" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
-      <c r="B7" s="33" t="s">
+    <row r="7" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="32"/>
+      <c r="B7" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="50" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="34" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
-      <c r="B8" s="33" t="s">
+    <row r="8" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="32"/>
+      <c r="B8" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="50" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="34" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
-      <c r="B9" s="26" t="s">
+    <row r="9" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="32"/>
+      <c r="B9" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="50" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="34" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="32" t="s">
+    <row r="10" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="50" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="34" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="32" t="s">
+    <row r="11" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="50" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="34" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="32" t="s">
+    <row r="12" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="50" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="34" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="32" t="s">
+    <row r="13" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="50" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="34" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="32" t="s">
+    <row r="14" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="32"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="50" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="34" customFormat="1" ht="39" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="32" t="s">
+    <row r="15" spans="1:3" s="31" customFormat="1" ht="38" x14ac:dyDescent="0.25">
+      <c r="A15" s="29"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="50" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="28" t="s">
+      <c r="A16" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="46" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="34"/>
+      <c r="B17" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="46" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="B18" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="41" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="46" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="36"/>
+      <c r="B20" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="46" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="36"/>
+      <c r="B21" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="46" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="36"/>
+      <c r="B22" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="46" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="37"/>
+      <c r="B23" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="46" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="41" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="44"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="41" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="45"/>
+      <c r="B26" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="41" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="B27" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="47" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="48"/>
+      <c r="B28" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="47" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="48"/>
+      <c r="B29" s="48"/>
+      <c r="C29" s="46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="48"/>
+      <c r="B30" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="46" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="48"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="47" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="48"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="46" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="48"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="46" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="38"/>
-      <c r="B17" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="37" t="s">
+    <row r="34" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="48"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="46" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="31" t="s">
+    <row r="35" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="48"/>
+      <c r="B35" s="48"/>
+      <c r="C35" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="33" t="s">
+    </row>
+    <row r="36" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="48"/>
+      <c r="B36" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" s="47" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19" s="37" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="40"/>
-      <c r="B20" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="37" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="40"/>
-      <c r="B21" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="C21" s="37" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="40"/>
-      <c r="B22" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="C22" s="37" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="41"/>
-      <c r="B23" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" s="37" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="26" t="s">
+    <row r="37" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="48"/>
+      <c r="B37" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="48"/>
+      <c r="B38" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="C24" s="33" t="s">
+      <c r="C38" s="47" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="48"/>
+      <c r="B39" s="33" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="48"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="33" t="s">
+      <c r="C39" s="47" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="49"/>
-      <c r="B26" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="C26" s="33" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="5"/>
-    </row>
-    <row r="29" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="5"/>
-    </row>
-    <row r="30" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="5"/>
-    </row>
-    <row r="31" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="5"/>
-    </row>
-    <row r="32" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="5"/>
-    </row>
-    <row r="33" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="5"/>
-    </row>
-    <row r="38" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="5" t="s">
+    <row r="40" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="48"/>
+      <c r="B40" s="48"/>
+      <c r="C40" s="46" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="48"/>
+      <c r="B41" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" s="49" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="48"/>
+      <c r="B42" s="48"/>
+      <c r="C42" s="46" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="48"/>
+      <c r="B43" s="48"/>
+      <c r="C43" s="46" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="48"/>
+      <c r="B44" s="48"/>
+      <c r="C44" s="46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="48"/>
+      <c r="B45" s="48"/>
+      <c r="C45" s="46" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="48"/>
+      <c r="B46" s="48"/>
+      <c r="C46" s="46" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="B47" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47" s="52" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="53"/>
+      <c r="B48" s="52" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="5" t="s">
-        <v>62</v>
-      </c>
+      <c r="C48" s="52" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="53"/>
+      <c r="B49" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49" s="52" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="53"/>
+      <c r="B50" s="53"/>
+      <c r="C50" s="52" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="53"/>
+      <c r="B51" s="53"/>
+      <c r="C51" s="41" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="53"/>
+      <c r="B52" s="53"/>
+      <c r="C52" s="41" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="53"/>
+      <c r="B53" s="53"/>
+      <c r="C53" s="41" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="53"/>
+      <c r="B54" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="52" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="53"/>
+      <c r="B55" s="51" t="s">
+        <v>15</v>
+      </c>
+      <c r="C55" s="52" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="53"/>
+      <c r="B56" s="53"/>
+      <c r="C56" s="41" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="53"/>
+      <c r="B57" s="53"/>
+      <c r="C57" s="41" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="53"/>
+      <c r="B58" s="53"/>
+      <c r="C58" s="41" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="30"/>
+    </row>
+    <row r="60" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="30"/>
+    </row>
+    <row r="61" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="30"/>
+    </row>
+    <row r="62" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="14">
+    <mergeCell ref="B41:B46"/>
+    <mergeCell ref="A27:A46"/>
+    <mergeCell ref="A47:A58"/>
+    <mergeCell ref="B49:B53"/>
+    <mergeCell ref="B55:B58"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="A24:A26"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="B39:B40"/>
     <mergeCell ref="A5:A15"/>
     <mergeCell ref="B9:B15"/>
     <mergeCell ref="A16:A17"/>
@@ -1366,71 +1587,71 @@
         <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>90</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>90</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="21"/>
       <c r="C4" s="2" t="s">
-        <v>91</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="2" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="2" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>83</v>
+      <c r="B7" s="18" t="s">
+        <v>52</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="20"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="8" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="2" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -1490,19 +1711,19 @@
         <v>39</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>93</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="2" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1538,41 +1759,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="23" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="21" t="s">
-        <v>95</v>
+      <c r="C2" s="23" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22" t="s">
-        <v>78</v>
+      <c r="A3" s="24"/>
+      <c r="B3" s="24" t="s">
+        <v>47</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>96</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="8" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1603,13 +1824,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="23" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1617,11 +1838,11 @@
       <c r="A2" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="21" t="s">
-        <v>75</v>
+      <c r="B2" s="23" t="s">
+        <v>44</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1631,207 +1852,318 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F9F2131-8A9C-2341-B42A-00CB44D66BE4}">
-  <dimension ref="A4:A24"/>
+  <dimension ref="A2:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A24"/>
+      <selection activeCell="A2" sqref="A2:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+    <row r="2" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="33" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+      <c r="B2" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="47" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="48"/>
+      <c r="B3" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="47" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="48"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="48"/>
+      <c r="B5" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="46" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="48"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="47" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="48"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="46" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="48"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="46" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="48"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="46" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="48"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="46" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="48"/>
+      <c r="B11" s="46" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
-        <v>62</v>
-      </c>
+      <c r="C11" s="47" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="48"/>
+      <c r="B12" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="48"/>
+      <c r="B13" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="47" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="48"/>
+      <c r="B14" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="47" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="48"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="46" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="48"/>
+      <c r="B16" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="49" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="48"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="46" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="48"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="46" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="48"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="48"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="46" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="48"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="46" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="5"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A2:A21"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B21"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6440110-0EB2-9743-9942-8B0A79C4C29B}">
-  <dimension ref="A10:A21"/>
+  <dimension ref="A2:C49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A21"/>
+      <selection activeCell="B2" sqref="A2:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
-        <v>74</v>
-      </c>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="15"/>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="15"/>
+      <c r="B4" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="15"/>
+      <c r="B9" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="15"/>
+      <c r="B10" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="5"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="5"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77804AF4-B0AB-1F47-A6D3-90F534B026A1}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <mergeCells count="3">
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="A2:A13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2117,23 +2449,23 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="16" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
+      <c r="A3" s="17"/>
       <c r="B3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2184,10 +2516,10 @@
         <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2235,7 +2567,7 @@
         <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>32</v>
@@ -2253,7 +2585,7 @@
     <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="2" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>34</v>
@@ -2262,7 +2594,7 @@
     <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="2" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>36</v>
@@ -2271,7 +2603,7 @@
     <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="2" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>35</v>
@@ -2336,27 +2668,27 @@
       <c r="A2" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>83</v>
+      <c r="B2" s="18" t="s">
+        <v>52</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="11"/>
-      <c r="B3" s="17"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="8" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="2" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
shared GO term table
</commit_message>
<xml_diff>
--- a/Output/SuppTables/Shared_GO.xlsx
+++ b/Output/SuppTables/Shared_GO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jillashey/Desktop/PutnamLab/Repositories/SedimentStress/SedimentStress/Output/SuppTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F704D710-C99F-CB4D-9756-6F2F207D4EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8247F142-74D9-0A42-889B-026F9C051A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16520" yWindow="500" windowWidth="19320" windowHeight="20740" xr2:uid="{463EAF44-39AF-B74B-A9CF-96AD4C6642C9}"/>
+    <workbookView xWindow="14360" yWindow="500" windowWidth="21480" windowHeight="20360" xr2:uid="{463EAF44-39AF-B74B-A9CF-96AD4C6642C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Full" sheetId="17" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="124">
   <si>
     <t>A.cervicornis + M.cavernosa + M.capitata</t>
   </si>
@@ -63,6 +63,15 @@
     <t xml:space="preserve">A.cervicornis + M.cavernosa </t>
   </si>
   <si>
+    <t>A.cervicornis + O.faveolata</t>
+  </si>
+  <si>
+    <t>M.capitata + P.acuta</t>
+  </si>
+  <si>
+    <t>P.acuta + P.lobata</t>
+  </si>
+  <si>
     <t>positive regulation of skeletal muscle tissue development (GO:0048643)</t>
   </si>
   <si>
@@ -378,24 +387,6 @@
     <t>negative regulation of cardiac cell fate specification (GO:2000044)</t>
   </si>
   <si>
-    <t xml:space="preserve">Averv + Ofav </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acerv + Mcap </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acerv + Pacuta </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acerv + Plob </t>
-  </si>
-  <si>
-    <t>Mcap + Pacuta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pacuta + Plob </t>
-  </si>
-  <si>
     <t>maintenance of gastrointestinal epithelium (GO:0030277)</t>
   </si>
   <si>
@@ -409,13 +400,203 @@
   </si>
   <si>
     <t>mesenchymal stem cell maintenance involved in nephron morphogenesis (GO:0072038)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>A.cervicornis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>M.cavernosa</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>M.capitata</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">M.capitata </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>M.cavernosa</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>P.acuta</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>M.capitata</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>P.acuta</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>P.lobata</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>A.cervicornis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">M.cavernosa </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">A.cervicornis + M.capitata  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.cervicornis + P.acuta </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.cervicornis +  P.lobata </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -473,6 +654,26 @@
       <b/>
       <sz val="18"/>
       <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -561,7 +762,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -611,6 +812,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -645,18 +847,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -672,12 +862,6 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -696,10 +880,46 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1016,523 +1236,581 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{113029E7-F384-C24D-A58A-6D6AAA957483}">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="56" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.5" style="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35" style="39" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="112" style="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="30"/>
+    <col min="1" max="1" width="45.5" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35" style="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="112" style="37" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="25" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:4" s="26" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="57"/>
+    </row>
+    <row r="2" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="D2" s="36"/>
+    </row>
+    <row r="3" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="40" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="36"/>
+    </row>
+    <row r="4" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="36"/>
+    </row>
+    <row r="5" spans="1:4" s="32" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="58"/>
+    </row>
+    <row r="6" spans="1:4" s="32" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="33"/>
+      <c r="B6" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="58"/>
+    </row>
+    <row r="7" spans="1:4" s="32" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="33"/>
+      <c r="B7" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="58"/>
+    </row>
+    <row r="8" spans="1:4" s="32" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="33"/>
+      <c r="B8" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="58"/>
+    </row>
+    <row r="9" spans="1:4" s="32" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="33"/>
+      <c r="B9" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="58"/>
+    </row>
+    <row r="10" spans="1:4" s="32" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="33"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="58"/>
+    </row>
+    <row r="11" spans="1:4" s="32" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="33"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="58"/>
+    </row>
+    <row r="12" spans="1:4" s="32" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="33"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="58"/>
+    </row>
+    <row r="13" spans="1:4" s="32" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="33"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="58"/>
+    </row>
+    <row r="14" spans="1:4" s="32" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="33"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="58"/>
+    </row>
+    <row r="15" spans="1:4" s="32" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A15" s="30"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="58"/>
+    </row>
+    <row r="16" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="36"/>
+    </row>
+    <row r="17" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="48"/>
+      <c r="B17" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="36"/>
+    </row>
+    <row r="18" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="49" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="36"/>
+    </row>
+    <row r="19" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" s="36"/>
+    </row>
+    <row r="20" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="51"/>
+      <c r="B20" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="D20" s="36"/>
+    </row>
+    <row r="21" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="51"/>
+      <c r="B21" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" s="36"/>
+    </row>
+    <row r="22" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="51"/>
+      <c r="B22" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="D22" s="36"/>
+    </row>
+    <row r="23" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="52"/>
+      <c r="B23" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="D23" s="36"/>
+    </row>
+    <row r="24" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="53" t="s">
+        <v>123</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="36"/>
+    </row>
+    <row r="25" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="54"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="36"/>
+    </row>
+    <row r="26" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="55"/>
+      <c r="B26" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="36"/>
+    </row>
+    <row r="27" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="B27" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="36"/>
+    </row>
+    <row r="28" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="48"/>
+      <c r="B28" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="36"/>
+    </row>
+    <row r="29" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="48"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" s="36"/>
+    </row>
+    <row r="30" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="48"/>
+      <c r="B30" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" s="36"/>
+    </row>
+    <row r="31" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="48"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="36"/>
+    </row>
+    <row r="32" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="48"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="D32" s="36"/>
+    </row>
+    <row r="33" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="48"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" s="36"/>
+    </row>
+    <row r="34" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="48"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" s="36"/>
+    </row>
+    <row r="35" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="48"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="D35" s="36"/>
+    </row>
+    <row r="36" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="48"/>
+      <c r="B36" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="D36" s="36"/>
+    </row>
+    <row r="37" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="48"/>
+      <c r="B37" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" s="36"/>
+    </row>
+    <row r="38" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="48"/>
+      <c r="B38" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="C38" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" s="36"/>
+    </row>
+    <row r="39" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="48"/>
+      <c r="B39" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="C39" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="D39" s="36"/>
+    </row>
+    <row r="40" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="48"/>
+      <c r="B40" s="35"/>
+      <c r="C40" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="D40" s="36"/>
+    </row>
+    <row r="41" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="48"/>
+      <c r="B41" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="D41" s="36"/>
+    </row>
+    <row r="42" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="48"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="D42" s="36"/>
+    </row>
+    <row r="43" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="48"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="D43" s="36"/>
+    </row>
+    <row r="44" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="48"/>
+      <c r="B44" s="35"/>
+      <c r="C44" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="D44" s="36"/>
+    </row>
+    <row r="45" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="48"/>
+      <c r="B45" s="35"/>
+      <c r="C45" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="D45" s="36"/>
+    </row>
+    <row r="46" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="48"/>
+      <c r="B46" s="35"/>
+      <c r="C46" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="D46" s="36"/>
+    </row>
+    <row r="47" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="56" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="47" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="50" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="42" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="47" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="50" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
-      <c r="B6" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="50" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
-      <c r="B7" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="50" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
-      <c r="B8" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="50" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="50" t="s">
+      <c r="B47" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="C47" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="D47" s="23"/>
+    </row>
+    <row r="48" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="59"/>
+      <c r="B48" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="C48" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="D48" s="23"/>
+    </row>
+    <row r="49" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="59"/>
+      <c r="B49" s="46" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="D49" s="23"/>
+    </row>
+    <row r="50" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="59"/>
+      <c r="B50" s="60"/>
+      <c r="C50" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="D50" s="23"/>
+    </row>
+    <row r="51" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="59"/>
+      <c r="B51" s="60"/>
+      <c r="C51" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="D51" s="23"/>
+    </row>
+    <row r="52" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="59"/>
+      <c r="B52" s="60"/>
+      <c r="C52" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="D52" s="23"/>
+    </row>
+    <row r="53" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="59"/>
+      <c r="B53" s="60"/>
+      <c r="C53" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="D53" s="23"/>
+    </row>
+    <row r="54" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="59"/>
+      <c r="B54" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="C54" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="D54" s="23"/>
+    </row>
+    <row r="55" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="59"/>
+      <c r="B55" s="46" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="50" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="50" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="50" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="50" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="50" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" s="31" customFormat="1" ht="38" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="50" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="33" t="s">
+      <c r="C55" s="40" t="s">
+        <v>108</v>
+      </c>
+      <c r="D55" s="23"/>
+    </row>
+    <row r="56" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="59"/>
+      <c r="B56" s="60"/>
+      <c r="C56" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="B16" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="46" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="34"/>
-      <c r="B17" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="46" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="41" t="s">
+      <c r="D56" s="23"/>
+    </row>
+    <row r="57" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="59"/>
+      <c r="B57" s="60"/>
+      <c r="C57" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="B18" s="43" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="41" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="35" t="s">
+      <c r="D57" s="23"/>
+    </row>
+    <row r="58" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="59"/>
+      <c r="B58" s="60"/>
+      <c r="C58" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="B19" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="46" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="36"/>
-      <c r="B20" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="46" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="36"/>
-      <c r="B21" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="46" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="36"/>
-      <c r="B22" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="46" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="37"/>
-      <c r="B23" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="46" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="B24" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="41" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="44"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="41" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="45"/>
-      <c r="B26" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="41" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="33" t="s">
-        <v>113</v>
-      </c>
-      <c r="B27" s="46" t="s">
-        <v>73</v>
-      </c>
-      <c r="C27" s="47" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="48"/>
-      <c r="B28" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="C28" s="47" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="48"/>
-      <c r="B29" s="48"/>
-      <c r="C29" s="46" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="48"/>
-      <c r="B30" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="C30" s="46" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="48"/>
-      <c r="B31" s="48"/>
-      <c r="C31" s="47" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="48"/>
-      <c r="B32" s="48"/>
-      <c r="C32" s="46" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="48"/>
-      <c r="B33" s="48"/>
-      <c r="C33" s="46" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="48"/>
-      <c r="B34" s="48"/>
-      <c r="C34" s="46" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="48"/>
-      <c r="B35" s="48"/>
-      <c r="C35" s="46" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="48"/>
-      <c r="B36" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="C36" s="47" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="48"/>
-      <c r="B37" s="46" t="s">
-        <v>69</v>
-      </c>
-      <c r="C37" s="47" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="48"/>
-      <c r="B38" s="46" t="s">
-        <v>83</v>
-      </c>
-      <c r="C38" s="47" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="48"/>
-      <c r="B39" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="C39" s="47" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="48"/>
-      <c r="B40" s="48"/>
-      <c r="C40" s="46" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="48"/>
-      <c r="B41" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="C41" s="49" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="48"/>
-      <c r="B42" s="48"/>
-      <c r="C42" s="46" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="48"/>
-      <c r="B43" s="48"/>
-      <c r="C43" s="46" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="48"/>
-      <c r="B44" s="48"/>
-      <c r="C44" s="46" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="48"/>
-      <c r="B45" s="48"/>
-      <c r="C45" s="46" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="48"/>
-      <c r="B46" s="48"/>
-      <c r="C46" s="46" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="51" t="s">
-        <v>114</v>
-      </c>
-      <c r="B47" s="41" t="s">
-        <v>95</v>
-      </c>
-      <c r="C47" s="52" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="53"/>
-      <c r="B48" s="52" t="s">
-        <v>53</v>
-      </c>
-      <c r="C48" s="52" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="53"/>
-      <c r="B49" s="51" t="s">
-        <v>98</v>
-      </c>
-      <c r="C49" s="52" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="53"/>
-      <c r="B50" s="53"/>
-      <c r="C50" s="52" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="53"/>
-      <c r="B51" s="53"/>
-      <c r="C51" s="41" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="53"/>
-      <c r="B52" s="53"/>
-      <c r="C52" s="41" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="53"/>
-      <c r="B53" s="53"/>
-      <c r="C53" s="41" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="53"/>
-      <c r="B54" s="41" t="s">
-        <v>103</v>
-      </c>
-      <c r="C54" s="52" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="53"/>
-      <c r="B55" s="51" t="s">
-        <v>15</v>
-      </c>
-      <c r="C55" s="52" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="53"/>
-      <c r="B56" s="53"/>
-      <c r="C56" s="41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="53"/>
-      <c r="B57" s="53"/>
-      <c r="C57" s="41" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="53"/>
-      <c r="B58" s="53"/>
-      <c r="C58" s="41" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="30"/>
-    </row>
-    <row r="60" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="30"/>
-    </row>
-    <row r="61" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="30"/>
-    </row>
-    <row r="62" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="30"/>
+      <c r="D58" s="23"/>
+    </row>
+    <row r="59" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D59" s="36"/>
+    </row>
+    <row r="60" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D60" s="36"/>
+    </row>
+    <row r="61" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D61" s="36"/>
+    </row>
+    <row r="62" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -1573,85 +1851,85 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
       <c r="B3" s="10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="20"/>
       <c r="B4" s="21"/>
       <c r="C4" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="20"/>
       <c r="B5" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
       <c r="B6" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="20"/>
       <c r="B8" s="22"/>
       <c r="C8" s="8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="21"/>
       <c r="B9" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -1697,33 +1975,33 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1759,41 +2037,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>6</v>
+      <c r="A1" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>64</v>
+        <v>43</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24" t="s">
-        <v>47</v>
+      <c r="A3" s="25"/>
+      <c r="B3" s="25" t="s">
+        <v>50</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="8" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1824,25 +2102,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>6</v>
+      <c r="A1" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="23" t="s">
         <v>44</v>
       </c>
+      <c r="B2" s="24" t="s">
+        <v>47</v>
+      </c>
       <c r="C2" s="8" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1860,162 +2138,162 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="46" t="s">
+    <row r="2" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="43"/>
+      <c r="B3" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C3" s="42" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48"/>
-      <c r="B3" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" s="47" t="s">
+    <row r="4" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="43"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="41" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="43"/>
+      <c r="B5" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="43"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="42" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="43"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="41" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="43"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="41" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="43"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="41" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="43"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="41" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="43"/>
+      <c r="B11" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="42" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="43"/>
+      <c r="B12" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="42" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="48"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="46" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="48"/>
-      <c r="B5" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="46" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="48"/>
-      <c r="B6" s="48"/>
-      <c r="C6" s="47" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="48"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="46" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="48"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="46" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="48"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="46" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="48"/>
-      <c r="B10" s="48"/>
-      <c r="C10" s="46" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="48"/>
-      <c r="B11" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="47" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="48"/>
-      <c r="B12" s="46" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" s="47" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="48"/>
-      <c r="B13" s="46" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" s="47" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="48"/>
-      <c r="B14" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="C14" s="47" t="s">
+    <row r="13" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="43"/>
+      <c r="B13" s="41" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="48"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="46" t="s">
+      <c r="C13" s="42" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="48"/>
-      <c r="B16" s="33" t="s">
+    <row r="14" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="43"/>
+      <c r="B14" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="49" t="s">
+      <c r="C14" s="42" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="48"/>
-      <c r="B17" s="48"/>
-      <c r="C17" s="46" t="s">
+    <row r="15" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="43"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="41" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="48"/>
-      <c r="B18" s="48"/>
-      <c r="C18" s="46" t="s">
+    <row r="16" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="43"/>
+      <c r="B16" s="34" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="48"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="46" t="s">
+      <c r="C16" s="44" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="48"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="46" t="s">
+    <row r="17" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="43"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="41" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="48"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="46" t="s">
+    <row r="18" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="43"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="41" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="43"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="43"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="41" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="43"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="41" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -2055,98 +2333,98 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="15"/>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="15"/>
       <c r="B4" s="14" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="15"/>
       <c r="B5" s="15"/>
       <c r="C5" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="15"/>
       <c r="B6" s="15"/>
       <c r="C6" s="5" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
       <c r="C7" s="5" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="15"/>
       <c r="B8" s="15"/>
       <c r="C8" s="5" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="15"/>
       <c r="B9" s="5" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C9" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="15"/>
       <c r="B10" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="15"/>
       <c r="B11" s="15"/>
       <c r="C11" s="5" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="15"/>
       <c r="B12" s="15"/>
       <c r="C12" s="5" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="15"/>
       <c r="B13" s="15"/>
       <c r="C13" s="5" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
@@ -2185,13 +2463,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -2199,10 +2477,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -2226,13 +2504,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="80" x14ac:dyDescent="0.25">
@@ -2240,10 +2518,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2269,13 +2547,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -2283,10 +2561,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2312,13 +2590,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2326,88 +2604,88 @@
         <v>3</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="8" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="8" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="10" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="12"/>
       <c r="C12" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="24" x14ac:dyDescent="0.3">
@@ -2439,33 +2717,33 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="17"/>
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2502,24 +2780,24 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2553,60 +2831,60 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2655,40 +2933,40 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="11"/>
       <c r="B3" s="19"/>
       <c r="C3" s="8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
editing tables while writing manuscript
</commit_message>
<xml_diff>
--- a/Output/SuppTables/Shared_GO.xlsx
+++ b/Output/SuppTables/Shared_GO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jillashey/Desktop/PutnamLab/Repositories/SedimentStress/SedimentStress/Output/SuppTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8247F142-74D9-0A42-889B-026F9C051A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B590287-E33A-8F43-80F5-EB2A9B1DB7E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14360" yWindow="500" windowWidth="21480" windowHeight="20360" xr2:uid="{463EAF44-39AF-B74B-A9CF-96AD4C6642C9}"/>
+    <workbookView xWindow="15560" yWindow="500" windowWidth="21480" windowHeight="20360" xr2:uid="{463EAF44-39AF-B74B-A9CF-96AD4C6642C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Full" sheetId="17" r:id="rId1"/>
@@ -777,6 +777,110 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -786,142 +890,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1238,596 +1238,596 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{113029E7-F384-C24D-A58A-6D6AAA957483}">
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35" style="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="112" style="37" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="31"/>
+    <col min="1" max="1" width="45.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="112" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="26" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:4" s="12" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="57"/>
+      <c r="D1" s="27"/>
     </row>
     <row r="2" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="36"/>
+      <c r="D2" s="17"/>
     </row>
     <row r="3" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="36"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="36"/>
-    </row>
-    <row r="5" spans="1:4" s="32" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="D4" s="17"/>
+    </row>
+    <row r="5" spans="1:4" s="16" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="37" t="s">
         <v>120</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="58"/>
-    </row>
-    <row r="6" spans="1:4" s="32" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="33"/>
-      <c r="B6" s="38" t="s">
+      <c r="D5" s="28"/>
+    </row>
+    <row r="6" spans="1:4" s="16" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="42"/>
+      <c r="B6" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="58"/>
-    </row>
-    <row r="7" spans="1:4" s="32" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
-      <c r="B7" s="38" t="s">
+      <c r="D6" s="28"/>
+    </row>
+    <row r="7" spans="1:4" s="16" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="42"/>
+      <c r="B7" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="58"/>
-    </row>
-    <row r="8" spans="1:4" s="32" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="33"/>
-      <c r="B8" s="38" t="s">
+      <c r="D7" s="28"/>
+    </row>
+    <row r="8" spans="1:4" s="16" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="42"/>
+      <c r="B8" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="58"/>
-    </row>
-    <row r="9" spans="1:4" s="32" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="B9" s="29" t="s">
+      <c r="D8" s="28"/>
+    </row>
+    <row r="9" spans="1:4" s="16" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="42"/>
+      <c r="B9" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="58"/>
-    </row>
-    <row r="10" spans="1:4" s="32" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="45" t="s">
+      <c r="D9" s="28"/>
+    </row>
+    <row r="10" spans="1:4" s="16" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="42"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="58"/>
-    </row>
-    <row r="11" spans="1:4" s="32" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="45" t="s">
+      <c r="D10" s="28"/>
+    </row>
+    <row r="11" spans="1:4" s="16" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="42"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="58"/>
-    </row>
-    <row r="12" spans="1:4" s="32" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="33"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="45" t="s">
+      <c r="D11" s="28"/>
+    </row>
+    <row r="12" spans="1:4" s="16" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="42"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="58"/>
-    </row>
-    <row r="13" spans="1:4" s="32" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="33"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="45" t="s">
+      <c r="D12" s="28"/>
+    </row>
+    <row r="13" spans="1:4" s="16" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="42"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="58"/>
-    </row>
-    <row r="14" spans="1:4" s="32" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="33"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="45" t="s">
+      <c r="D13" s="28"/>
+    </row>
+    <row r="14" spans="1:4" s="16" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="42"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="58"/>
-    </row>
-    <row r="15" spans="1:4" s="32" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="45" t="s">
+      <c r="D14" s="28"/>
+    </row>
+    <row r="15" spans="1:4" s="16" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A15" s="38"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="58"/>
+      <c r="D15" s="28"/>
     </row>
     <row r="16" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="41" t="s">
+      <c r="C16" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="36"/>
+      <c r="D16" s="17"/>
     </row>
     <row r="17" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="48"/>
-      <c r="B17" s="39" t="s">
+      <c r="A17" s="32"/>
+      <c r="B17" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="36"/>
+      <c r="D17" s="17"/>
     </row>
     <row r="18" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="49" t="s">
+      <c r="A18" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="38" t="s">
+      <c r="C18" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="36"/>
+      <c r="D18" s="17"/>
     </row>
     <row r="19" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="41" t="s">
+      <c r="C19" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="D19" s="36"/>
+      <c r="D19" s="17"/>
     </row>
     <row r="20" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="51"/>
-      <c r="B20" s="39" t="s">
+      <c r="A20" s="44"/>
+      <c r="B20" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="41" t="s">
+      <c r="C20" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="D20" s="36"/>
+      <c r="D20" s="17"/>
     </row>
     <row r="21" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="51"/>
-      <c r="B21" s="39" t="s">
+      <c r="A21" s="44"/>
+      <c r="B21" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="41" t="s">
+      <c r="C21" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="D21" s="36"/>
+      <c r="D21" s="17"/>
     </row>
     <row r="22" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="51"/>
-      <c r="B22" s="39" t="s">
+      <c r="A22" s="44"/>
+      <c r="B22" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="41" t="s">
+      <c r="C22" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="D22" s="36"/>
+      <c r="D22" s="17"/>
     </row>
     <row r="23" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="52"/>
-      <c r="B23" s="39" t="s">
+      <c r="A23" s="45"/>
+      <c r="B23" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="41" t="s">
+      <c r="C23" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="D23" s="36"/>
+      <c r="D23" s="17"/>
     </row>
     <row r="24" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="53" t="s">
+      <c r="A24" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="38" t="s">
+      <c r="C24" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="36"/>
+      <c r="D24" s="17"/>
     </row>
     <row r="25" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="54"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="38" t="s">
+      <c r="A25" s="40"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="D25" s="36"/>
+      <c r="D25" s="17"/>
     </row>
     <row r="26" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="55"/>
-      <c r="B26" s="40" t="s">
+      <c r="A26" s="41"/>
+      <c r="B26" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="38" t="s">
+      <c r="C26" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="D26" s="36"/>
+      <c r="D26" s="17"/>
     </row>
     <row r="27" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="47" t="s">
+      <c r="A27" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="41" t="s">
+      <c r="B27" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="C27" s="42" t="s">
+      <c r="C27" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="D27" s="36"/>
+      <c r="D27" s="17"/>
     </row>
     <row r="28" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="48"/>
-      <c r="B28" s="34" t="s">
+      <c r="A28" s="32"/>
+      <c r="B28" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="C28" s="42" t="s">
+      <c r="C28" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="D28" s="36"/>
+      <c r="D28" s="17"/>
     </row>
     <row r="29" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="48"/>
-      <c r="B29" s="35"/>
-      <c r="C29" s="41" t="s">
+      <c r="A29" s="32"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="D29" s="36"/>
+      <c r="D29" s="17"/>
     </row>
     <row r="30" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="48"/>
-      <c r="B30" s="34" t="s">
+      <c r="A30" s="32"/>
+      <c r="B30" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="C30" s="41" t="s">
+      <c r="C30" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="D30" s="36"/>
+      <c r="D30" s="17"/>
     </row>
     <row r="31" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="48"/>
-      <c r="B31" s="35"/>
-      <c r="C31" s="42" t="s">
+      <c r="A31" s="32"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="D31" s="36"/>
+      <c r="D31" s="17"/>
     </row>
     <row r="32" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="48"/>
-      <c r="B32" s="35"/>
-      <c r="C32" s="41" t="s">
+      <c r="A32" s="32"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="D32" s="36"/>
+      <c r="D32" s="17"/>
     </row>
     <row r="33" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="48"/>
-      <c r="B33" s="35"/>
-      <c r="C33" s="41" t="s">
+      <c r="A33" s="32"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="D33" s="36"/>
+      <c r="D33" s="17"/>
     </row>
     <row r="34" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="48"/>
-      <c r="B34" s="35"/>
-      <c r="C34" s="41" t="s">
+      <c r="A34" s="32"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="D34" s="36"/>
+      <c r="D34" s="17"/>
     </row>
     <row r="35" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="48"/>
-      <c r="B35" s="35"/>
-      <c r="C35" s="41" t="s">
+      <c r="A35" s="32"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="D35" s="36"/>
+      <c r="D35" s="17"/>
     </row>
     <row r="36" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="48"/>
-      <c r="B36" s="41" t="s">
+      <c r="A36" s="32"/>
+      <c r="B36" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="C36" s="42" t="s">
+      <c r="C36" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="D36" s="36"/>
+      <c r="D36" s="17"/>
     </row>
     <row r="37" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="48"/>
-      <c r="B37" s="41" t="s">
+      <c r="A37" s="32"/>
+      <c r="B37" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="42" t="s">
+      <c r="C37" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="36"/>
+      <c r="D37" s="17"/>
     </row>
     <row r="38" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="48"/>
-      <c r="B38" s="41" t="s">
+      <c r="A38" s="32"/>
+      <c r="B38" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="C38" s="42" t="s">
+      <c r="C38" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="D38" s="36"/>
+      <c r="D38" s="17"/>
     </row>
     <row r="39" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="48"/>
-      <c r="B39" s="34" t="s">
+      <c r="A39" s="32"/>
+      <c r="B39" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="C39" s="42" t="s">
+      <c r="C39" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="D39" s="36"/>
+      <c r="D39" s="17"/>
     </row>
     <row r="40" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="48"/>
-      <c r="B40" s="35"/>
-      <c r="C40" s="41" t="s">
+      <c r="A40" s="32"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="D40" s="36"/>
+      <c r="D40" s="17"/>
     </row>
     <row r="41" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="48"/>
-      <c r="B41" s="34" t="s">
+      <c r="A41" s="32"/>
+      <c r="B41" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C41" s="39" t="s">
+      <c r="C41" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="D41" s="36"/>
+      <c r="D41" s="17"/>
     </row>
     <row r="42" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="48"/>
-      <c r="B42" s="35"/>
-      <c r="C42" s="41" t="s">
+      <c r="A42" s="32"/>
+      <c r="B42" s="30"/>
+      <c r="C42" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="D42" s="36"/>
+      <c r="D42" s="17"/>
     </row>
     <row r="43" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="48"/>
-      <c r="B43" s="35"/>
-      <c r="C43" s="41" t="s">
+      <c r="A43" s="32"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="D43" s="36"/>
+      <c r="D43" s="17"/>
     </row>
     <row r="44" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="48"/>
-      <c r="B44" s="35"/>
-      <c r="C44" s="41" t="s">
+      <c r="A44" s="32"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="D44" s="36"/>
+      <c r="D44" s="17"/>
     </row>
     <row r="45" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="48"/>
-      <c r="B45" s="35"/>
-      <c r="C45" s="41" t="s">
+      <c r="A45" s="32"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="D45" s="36"/>
+      <c r="D45" s="17"/>
     </row>
     <row r="46" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="48"/>
-      <c r="B46" s="35"/>
-      <c r="C46" s="41" t="s">
+      <c r="A46" s="32"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="D46" s="36"/>
+      <c r="D46" s="17"/>
     </row>
     <row r="47" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="56" t="s">
+      <c r="A47" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="38" t="s">
+      <c r="B47" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="C47" s="40" t="s">
+      <c r="C47" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="D47" s="23"/>
+      <c r="D47" s="10"/>
     </row>
     <row r="48" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="59"/>
-      <c r="B48" s="40" t="s">
+      <c r="A48" s="34"/>
+      <c r="B48" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="C48" s="40" t="s">
+      <c r="C48" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="D48" s="23"/>
+      <c r="D48" s="10"/>
     </row>
     <row r="49" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="59"/>
-      <c r="B49" s="46" t="s">
+      <c r="A49" s="34"/>
+      <c r="B49" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="C49" s="40" t="s">
+      <c r="C49" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="D49" s="23"/>
+      <c r="D49" s="10"/>
     </row>
     <row r="50" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="59"/>
-      <c r="B50" s="60"/>
-      <c r="C50" s="40" t="s">
+      <c r="A50" s="34"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="D50" s="23"/>
+      <c r="D50" s="10"/>
     </row>
     <row r="51" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="59"/>
-      <c r="B51" s="60"/>
-      <c r="C51" s="38" t="s">
+      <c r="A51" s="34"/>
+      <c r="B51" s="36"/>
+      <c r="C51" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="D51" s="23"/>
+      <c r="D51" s="10"/>
     </row>
     <row r="52" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="59"/>
-      <c r="B52" s="60"/>
-      <c r="C52" s="38" t="s">
+      <c r="A52" s="34"/>
+      <c r="B52" s="36"/>
+      <c r="C52" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="D52" s="23"/>
+      <c r="D52" s="10"/>
     </row>
     <row r="53" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="59"/>
-      <c r="B53" s="60"/>
-      <c r="C53" s="38" t="s">
+      <c r="A53" s="34"/>
+      <c r="B53" s="36"/>
+      <c r="C53" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="D53" s="23"/>
+      <c r="D53" s="10"/>
     </row>
     <row r="54" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="59"/>
-      <c r="B54" s="38" t="s">
+      <c r="A54" s="34"/>
+      <c r="B54" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="C54" s="40" t="s">
+      <c r="C54" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="D54" s="23"/>
+      <c r="D54" s="10"/>
     </row>
     <row r="55" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="59"/>
-      <c r="B55" s="46" t="s">
+      <c r="A55" s="34"/>
+      <c r="B55" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C55" s="40" t="s">
+      <c r="C55" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="D55" s="23"/>
+      <c r="D55" s="10"/>
     </row>
     <row r="56" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="59"/>
-      <c r="B56" s="60"/>
-      <c r="C56" s="38" t="s">
+      <c r="A56" s="34"/>
+      <c r="B56" s="36"/>
+      <c r="C56" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="D56" s="23"/>
+      <c r="D56" s="10"/>
     </row>
     <row r="57" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="59"/>
-      <c r="B57" s="60"/>
-      <c r="C57" s="38" t="s">
+      <c r="A57" s="34"/>
+      <c r="B57" s="36"/>
+      <c r="C57" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="D57" s="23"/>
+      <c r="D57" s="10"/>
     </row>
     <row r="58" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="59"/>
-      <c r="B58" s="60"/>
-      <c r="C58" s="38" t="s">
+      <c r="A58" s="34"/>
+      <c r="B58" s="36"/>
+      <c r="C58" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="D58" s="23"/>
+      <c r="D58" s="10"/>
     </row>
     <row r="59" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D59" s="36"/>
+      <c r="D59" s="17"/>
     </row>
     <row r="60" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D60" s="36"/>
+      <c r="D60" s="17"/>
     </row>
     <row r="61" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D61" s="36"/>
+      <c r="D61" s="17"/>
     </row>
     <row r="62" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="31"/>
+      <c r="A62" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A5:A15"/>
+    <mergeCell ref="B9:B15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="B39:B40"/>
     <mergeCell ref="B41:B46"/>
     <mergeCell ref="A27:A46"/>
     <mergeCell ref="A47:A58"/>
     <mergeCell ref="B49:B53"/>
     <mergeCell ref="B55:B58"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B30:B35"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A5:A15"/>
-    <mergeCell ref="B9:B15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A19:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1861,7 +1861,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="51" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1872,8 +1872,8 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="10" t="s">
+      <c r="A3" s="55"/>
+      <c r="B3" s="46" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1881,14 +1881,14 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="21"/>
+      <c r="A4" s="55"/>
+      <c r="B4" s="54"/>
       <c r="C4" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
+      <c r="A5" s="55"/>
       <c r="B5" s="2" t="s">
         <v>59</v>
       </c>
@@ -1897,7 +1897,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
+      <c r="A6" s="54"/>
       <c r="B6" s="2" t="s">
         <v>50</v>
       </c>
@@ -1906,10 +1906,10 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="52" t="s">
         <v>55</v>
       </c>
       <c r="C7" s="8" t="s">
@@ -1917,14 +1917,14 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="22"/>
+      <c r="A8" s="55"/>
+      <c r="B8" s="56"/>
       <c r="C8" s="8" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
+      <c r="A9" s="54"/>
       <c r="B9" s="2" t="s">
         <v>56</v>
       </c>
@@ -1985,7 +1985,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="51" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -1996,7 +1996,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
+      <c r="A3" s="48"/>
       <c r="B3" s="2" t="s">
         <v>50</v>
       </c>
@@ -2037,30 +2037,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="11" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25" t="s">
+      <c r="A3" s="57"/>
+      <c r="B3" s="57" t="s">
         <v>50</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -2068,8 +2068,8 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
+      <c r="A4" s="57"/>
+      <c r="B4" s="57"/>
       <c r="C4" s="8" t="s">
         <v>69</v>
       </c>
@@ -2102,13 +2102,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="11" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2116,7 +2116,7 @@
       <c r="A2" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="11" t="s">
         <v>47</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -2138,161 +2138,161 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
+    <row r="2" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="23" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="43"/>
-      <c r="B3" s="34" t="s">
+    <row r="3" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="58"/>
+      <c r="B3" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="23" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="43"/>
-      <c r="B4" s="43"/>
-      <c r="C4" s="41" t="s">
+    <row r="4" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="58"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="22" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="43"/>
-      <c r="B5" s="34" t="s">
+    <row r="5" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="58"/>
+      <c r="B5" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="22" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="43"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="42" t="s">
+    <row r="6" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="58"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="23" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="43"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="41" t="s">
+    <row r="7" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="58"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="22" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="43"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="41" t="s">
+    <row r="8" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="58"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="22" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="43"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="41" t="s">
+    <row r="9" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="58"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="22" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="43"/>
-      <c r="B10" s="43"/>
-      <c r="C10" s="41" t="s">
+    <row r="10" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="58"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="22" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="43"/>
-      <c r="B11" s="41" t="s">
+    <row r="11" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="58"/>
+      <c r="B11" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="23" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="43"/>
-      <c r="B12" s="41" t="s">
+    <row r="12" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="58"/>
+      <c r="B12" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="23" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="43"/>
-      <c r="B13" s="41" t="s">
+    <row r="13" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="58"/>
+      <c r="B13" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="42" t="s">
+      <c r="C13" s="23" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="43"/>
-      <c r="B14" s="34" t="s">
+    <row r="14" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="58"/>
+      <c r="B14" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="23" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="43"/>
-      <c r="B15" s="43"/>
-      <c r="C15" s="41" t="s">
+    <row r="15" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="58"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="22" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="43"/>
-      <c r="B16" s="34" t="s">
+    <row r="16" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="58"/>
+      <c r="B16" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="24" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="43"/>
-      <c r="B17" s="43"/>
-      <c r="C17" s="41" t="s">
+    <row r="17" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="58"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="22" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="43"/>
-      <c r="B18" s="43"/>
-      <c r="C18" s="41" t="s">
+    <row r="18" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="58"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="22" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="43"/>
-      <c r="B19" s="43"/>
-      <c r="C19" s="41" t="s">
+    <row r="19" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="58"/>
+      <c r="B19" s="58"/>
+      <c r="C19" s="22" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="43"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="41" t="s">
+    <row r="20" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="58"/>
+      <c r="B20" s="58"/>
+      <c r="C20" s="22" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="31" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="43"/>
-      <c r="B21" s="43"/>
-      <c r="C21" s="41" t="s">
+    <row r="21" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="58"/>
+      <c r="B21" s="58"/>
+      <c r="C21" s="22" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2332,7 +2332,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="59" t="s">
         <v>46</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -2343,7 +2343,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="15"/>
+      <c r="A3" s="60"/>
       <c r="B3" t="s">
         <v>56</v>
       </c>
@@ -2352,8 +2352,8 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
-      <c r="B4" s="14" t="s">
+      <c r="A4" s="60"/>
+      <c r="B4" s="59" t="s">
         <v>101</v>
       </c>
       <c r="C4" t="s">
@@ -2361,35 +2361,35 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
+      <c r="A5" s="60"/>
+      <c r="B5" s="60"/>
       <c r="C5" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
+      <c r="A6" s="60"/>
+      <c r="B6" s="60"/>
       <c r="C6" s="5" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
+      <c r="A7" s="60"/>
+      <c r="B7" s="60"/>
       <c r="C7" s="5" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
+      <c r="A8" s="60"/>
+      <c r="B8" s="60"/>
       <c r="C8" s="5" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
+      <c r="A9" s="60"/>
       <c r="B9" s="5" t="s">
         <v>106</v>
       </c>
@@ -2398,8 +2398,8 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="15"/>
-      <c r="B10" s="14" t="s">
+      <c r="A10" s="60"/>
+      <c r="B10" s="59" t="s">
         <v>91</v>
       </c>
       <c r="C10" t="s">
@@ -2407,22 +2407,22 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
+      <c r="A11" s="60"/>
+      <c r="B11" s="60"/>
       <c r="C11" s="5" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
+      <c r="A12" s="60"/>
+      <c r="B12" s="60"/>
       <c r="C12" s="5" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
+      <c r="A13" s="60"/>
+      <c r="B13" s="60"/>
       <c r="C13" s="5" t="s">
         <v>111</v>
       </c>
@@ -2600,7 +2600,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="46" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -2611,7 +2611,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
+      <c r="A3" s="47"/>
       <c r="B3" s="8" t="s">
         <v>17</v>
       </c>
@@ -2620,7 +2620,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
+      <c r="A4" s="47"/>
       <c r="B4" s="8" t="s">
         <v>19</v>
       </c>
@@ -2629,7 +2629,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="A5" s="47"/>
       <c r="B5" s="8" t="s">
         <v>20</v>
       </c>
@@ -2638,8 +2638,8 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="10" t="s">
+      <c r="A6" s="47"/>
+      <c r="B6" s="46" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -2647,43 +2647,43 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
+      <c r="A7" s="47"/>
+      <c r="B7" s="47"/>
       <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
+      <c r="A8" s="47"/>
+      <c r="B8" s="47"/>
       <c r="C8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
+      <c r="A9" s="47"/>
+      <c r="B9" s="47"/>
       <c r="C9" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
+      <c r="A10" s="47"/>
+      <c r="B10" s="47"/>
       <c r="C10" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
+      <c r="A11" s="47"/>
+      <c r="B11" s="47"/>
       <c r="C11" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
+      <c r="A12" s="48"/>
+      <c r="B12" s="48"/>
       <c r="C12" s="2" t="s">
         <v>29</v>
       </c>
@@ -2727,7 +2727,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="49" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2738,7 +2738,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
+      <c r="A3" s="50"/>
       <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
@@ -2841,7 +2841,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="51" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2852,7 +2852,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
+      <c r="A3" s="47"/>
       <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
@@ -2861,7 +2861,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
+      <c r="A4" s="47"/>
       <c r="B4" s="2" t="s">
         <v>48</v>
       </c>
@@ -2870,7 +2870,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="A5" s="47"/>
       <c r="B5" s="2" t="s">
         <v>49</v>
       </c>
@@ -2879,7 +2879,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
+      <c r="A6" s="48"/>
       <c r="B6" s="2" t="s">
         <v>50</v>
       </c>
@@ -2943,10 +2943,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="52" t="s">
         <v>55</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -2954,14 +2954,14 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="11"/>
-      <c r="B3" s="19"/>
+      <c r="A3" s="47"/>
+      <c r="B3" s="53"/>
       <c r="C3" s="8" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
+      <c r="A4" s="48"/>
       <c r="B4" s="2" t="s">
         <v>56</v>
       </c>

</xml_diff>

<commit_message>
cleaning up output files
</commit_message>
<xml_diff>
--- a/Output/SuppTables/Shared_GO.xlsx
+++ b/Output/SuppTables/Shared_GO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jillashey/Desktop/PutnamLab/Repositories/SedimentStress/SedimentStress/Output/SuppTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B590287-E33A-8F43-80F5-EB2A9B1DB7E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F598F43-07BA-B342-A9E1-83170C1132C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15560" yWindow="500" windowWidth="21480" windowHeight="20360" xr2:uid="{463EAF44-39AF-B74B-A9CF-96AD4C6642C9}"/>
+    <workbookView xWindow="16960" yWindow="660" windowWidth="18260" windowHeight="20360" xr2:uid="{463EAF44-39AF-B74B-A9CF-96AD4C6642C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Full" sheetId="17" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="137">
   <si>
     <t>A.cervicornis + M.cavernosa + M.capitata</t>
   </si>
@@ -590,6 +590,45 @@
   </si>
   <si>
     <t xml:space="preserve">A.cervicornis +  P.lobata </t>
+  </si>
+  <si>
+    <t>GO slim Category</t>
+  </si>
+  <si>
+    <t>A.cervicornis</t>
+  </si>
+  <si>
+    <t>M. capitata</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> M.cavernosa </t>
+  </si>
+  <si>
+    <t>O.faveolata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P.acuta </t>
+  </si>
+  <si>
+    <t xml:space="preserve">P.lobata </t>
+  </si>
+  <si>
+    <t>See Supplementary Table xx</t>
+  </si>
+  <si>
+    <t>Number of shared GO terms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M.capitata + M.cavernosa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M.cavernosa + P.acuta </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M.cavernosa + P.lobata </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O.faveolata + P.acuta </t>
   </si>
 </sst>
 </file>
@@ -698,7 +737,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -758,11 +797,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -788,12 +853,21 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -821,6 +895,9 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -830,10 +907,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -922,6 +1002,91 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1236,598 +1401,884 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{113029E7-F384-C24D-A58A-6D6AAA957483}">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="B31" zoomScale="91" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="112" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="15"/>
+    <col min="1" max="1" width="45.5" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="35" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="112" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="12" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="12" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="14" t="s">
+      <c r="B1" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="27"/>
-    </row>
-    <row r="2" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
+      <c r="E1" s="31"/>
+    </row>
+    <row r="2" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="23">
+        <v>1</v>
+      </c>
+      <c r="C2" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="D2" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="17"/>
-    </row>
-    <row r="3" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="E2" s="20"/>
+    </row>
+    <row r="3" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="34">
+        <v>1</v>
+      </c>
+      <c r="C3" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="D3" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="17"/>
-    </row>
-    <row r="4" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="23">
+        <v>1</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="D4" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="17"/>
-    </row>
-    <row r="5" spans="1:4" s="16" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
+      <c r="E4" s="20"/>
+    </row>
+    <row r="5" spans="1:5" s="18" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="15"/>
+      <c r="C5" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="D5" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="28"/>
-    </row>
-    <row r="6" spans="1:4" s="16" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="42"/>
-      <c r="B6" s="19" t="s">
+      <c r="E5" s="32"/>
+    </row>
+    <row r="6" spans="1:5" s="18" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="47"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="D6" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="28"/>
-    </row>
-    <row r="7" spans="1:4" s="16" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="42"/>
-      <c r="B7" s="19" t="s">
+      <c r="E6" s="32"/>
+    </row>
+    <row r="7" spans="1:5" s="18" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="47"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="D7" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="28"/>
-    </row>
-    <row r="8" spans="1:4" s="16" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="42"/>
-      <c r="B8" s="19" t="s">
+      <c r="E7" s="32"/>
+    </row>
+    <row r="8" spans="1:5" s="18" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="47"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="D8" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="28"/>
-    </row>
-    <row r="9" spans="1:4" s="16" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="42"/>
-      <c r="B9" s="37" t="s">
+      <c r="E8" s="32"/>
+    </row>
+    <row r="9" spans="1:5" s="18" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="47"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="D9" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="28"/>
-    </row>
-    <row r="10" spans="1:4" s="16" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="42"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="25" t="s">
+      <c r="E9" s="32"/>
+    </row>
+    <row r="10" spans="1:5" s="18" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="47"/>
+      <c r="B10" s="19">
+        <v>11</v>
+      </c>
+      <c r="C10" s="47"/>
+      <c r="D10" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="28"/>
-    </row>
-    <row r="11" spans="1:4" s="16" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="42"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="25" t="s">
+      <c r="E10" s="32"/>
+    </row>
+    <row r="11" spans="1:5" s="18" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="47"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="28"/>
-    </row>
-    <row r="12" spans="1:4" s="16" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="42"/>
-      <c r="B12" s="42"/>
-      <c r="C12" s="25" t="s">
+      <c r="E11" s="32"/>
+    </row>
+    <row r="12" spans="1:5" s="18" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="47"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="28"/>
-    </row>
-    <row r="13" spans="1:4" s="16" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="42"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="25" t="s">
+      <c r="E12" s="32"/>
+    </row>
+    <row r="13" spans="1:5" s="18" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="47"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="28"/>
-    </row>
-    <row r="14" spans="1:4" s="16" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="42"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="25" t="s">
+      <c r="E13" s="32"/>
+    </row>
+    <row r="14" spans="1:5" s="18" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="47"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="28"/>
-    </row>
-    <row r="15" spans="1:4" s="16" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A15" s="38"/>
-      <c r="B15" s="38"/>
-      <c r="C15" s="25" t="s">
+      <c r="E14" s="32"/>
+    </row>
+    <row r="15" spans="1:5" s="18" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A15" s="43"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="28"/>
-    </row>
-    <row r="16" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="31" t="s">
+      <c r="E15" s="32"/>
+    </row>
+    <row r="16" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="70">
+        <v>2</v>
+      </c>
+      <c r="C16" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="D16" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="17"/>
-    </row>
-    <row r="17" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="32"/>
-      <c r="B17" s="20" t="s">
+      <c r="E16" s="20"/>
+    </row>
+    <row r="17" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="37"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="D17" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="17"/>
-    </row>
-    <row r="18" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="26" t="s">
+      <c r="E17" s="20"/>
+    </row>
+    <row r="18" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="29">
+        <v>1</v>
+      </c>
+      <c r="C18" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="D18" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="17"/>
-    </row>
-    <row r="19" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="43" t="s">
+      <c r="E18" s="20"/>
+    </row>
+    <row r="19" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="70">
+        <v>5</v>
+      </c>
+      <c r="C19" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="D19" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="D19" s="17"/>
-    </row>
-    <row r="20" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="44"/>
-      <c r="B20" s="20" t="s">
+      <c r="E19" s="20"/>
+    </row>
+    <row r="20" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="49"/>
+      <c r="B20" s="89"/>
+      <c r="C20" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="D20" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="D20" s="17"/>
-    </row>
-    <row r="21" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="44"/>
-      <c r="B21" s="20" t="s">
+      <c r="E20" s="20"/>
+    </row>
+    <row r="21" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="49"/>
+      <c r="B21" s="89"/>
+      <c r="C21" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="D21" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="D21" s="17"/>
-    </row>
-    <row r="22" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="44"/>
-      <c r="B22" s="20" t="s">
+      <c r="E21" s="20"/>
+    </row>
+    <row r="22" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="49"/>
+      <c r="B22" s="89"/>
+      <c r="C22" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="D22" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="D22" s="17"/>
-    </row>
-    <row r="23" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="45"/>
-      <c r="B23" s="20" t="s">
+      <c r="E22" s="20"/>
+    </row>
+    <row r="23" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="50"/>
+      <c r="B23" s="88"/>
+      <c r="C23" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="D23" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="D23" s="17"/>
-    </row>
-    <row r="24" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="39" t="s">
+      <c r="E23" s="20"/>
+    </row>
+    <row r="24" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="90"/>
+      <c r="C24" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="D24" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="17"/>
-    </row>
-    <row r="25" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="40"/>
-      <c r="B25" s="38"/>
-      <c r="C25" s="19" t="s">
+      <c r="E24" s="20"/>
+    </row>
+    <row r="25" spans="1:5" s="76" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="45"/>
+      <c r="B25" s="91">
+        <v>3</v>
+      </c>
+      <c r="C25" s="43"/>
+      <c r="D25" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="D25" s="17"/>
-    </row>
-    <row r="26" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="41"/>
-      <c r="B26" s="21" t="s">
+    </row>
+    <row r="26" spans="1:5" s="76" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="46"/>
+      <c r="B26" s="92"/>
+      <c r="C26" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="D26" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="D26" s="17"/>
-    </row>
-    <row r="27" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="31" t="s">
+    </row>
+    <row r="27" spans="1:5" s="76" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="48" t="s">
+        <v>133</v>
+      </c>
+      <c r="B27" s="70">
+        <v>4</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="76" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="49"/>
+      <c r="B28" s="79"/>
+      <c r="C28" s="80" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="76" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="49"/>
+      <c r="B29" s="79"/>
+      <c r="C29" s="73"/>
+      <c r="D29" s="23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="76" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="49"/>
+      <c r="B30" s="79"/>
+      <c r="C30" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="76" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="50"/>
+      <c r="B31" s="73"/>
+      <c r="C31" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="76" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B32" s="93">
+        <v>20</v>
+      </c>
+      <c r="C32" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="C27" s="23" t="s">
+      <c r="D32" s="87" t="s">
         <v>77</v>
       </c>
-      <c r="D27" s="17"/>
-    </row>
-    <row r="28" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="32"/>
-      <c r="B28" s="29" t="s">
+    </row>
+    <row r="33" spans="1:5" s="76" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="39"/>
+      <c r="B33" s="94"/>
+      <c r="C33" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="D33" s="87" t="s">
         <v>74</v>
       </c>
-      <c r="D28" s="17"/>
-    </row>
-    <row r="29" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="32"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="22" t="s">
+    </row>
+    <row r="34" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="39"/>
+      <c r="B34" s="94"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="D29" s="17"/>
-    </row>
-    <row r="30" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="32"/>
-      <c r="B30" s="29" t="s">
+      <c r="E34" s="20"/>
+    </row>
+    <row r="35" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="39"/>
+      <c r="B35" s="94"/>
+      <c r="C35" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="C30" s="22" t="s">
+      <c r="D35" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="D30" s="17"/>
-    </row>
-    <row r="31" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="32"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="23" t="s">
+      <c r="E35" s="20"/>
+    </row>
+    <row r="36" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="39"/>
+      <c r="B36" s="94"/>
+      <c r="C36" s="41"/>
+      <c r="D36" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="D31" s="17"/>
-    </row>
-    <row r="32" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="32"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="22" t="s">
+      <c r="E36" s="20"/>
+    </row>
+    <row r="37" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="39"/>
+      <c r="B37" s="94"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="D32" s="17"/>
-    </row>
-    <row r="33" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="32"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="22" t="s">
+      <c r="E37" s="20"/>
+    </row>
+    <row r="38" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="39"/>
+      <c r="B38" s="94"/>
+      <c r="C38" s="41"/>
+      <c r="D38" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="D33" s="17"/>
-    </row>
-    <row r="34" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="32"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="22" t="s">
+      <c r="E38" s="20"/>
+    </row>
+    <row r="39" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="39"/>
+      <c r="B39" s="94"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="D34" s="17"/>
-    </row>
-    <row r="35" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="32"/>
-      <c r="B35" s="30"/>
-      <c r="C35" s="22" t="s">
+      <c r="E39" s="20"/>
+    </row>
+    <row r="40" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="39"/>
+      <c r="B40" s="94"/>
+      <c r="C40" s="41"/>
+      <c r="D40" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="D35" s="17"/>
-    </row>
-    <row r="36" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="32"/>
-      <c r="B36" s="22" t="s">
+      <c r="E40" s="20"/>
+    </row>
+    <row r="41" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="39"/>
+      <c r="B41" s="94"/>
+      <c r="C41" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="C36" s="23" t="s">
+      <c r="D41" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D36" s="17"/>
-    </row>
-    <row r="37" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="32"/>
-      <c r="B37" s="22" t="s">
+      <c r="E41" s="20"/>
+    </row>
+    <row r="42" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="39"/>
+      <c r="B42" s="94"/>
+      <c r="C42" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="23" t="s">
+      <c r="D42" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="17"/>
-    </row>
-    <row r="38" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="32"/>
-      <c r="B38" s="22" t="s">
+      <c r="E42" s="20"/>
+    </row>
+    <row r="43" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="39"/>
+      <c r="B43" s="94"/>
+      <c r="C43" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="C38" s="23" t="s">
+      <c r="D43" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="D38" s="17"/>
-    </row>
-    <row r="39" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="32"/>
-      <c r="B39" s="29" t="s">
+      <c r="E43" s="20"/>
+    </row>
+    <row r="44" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="39"/>
+      <c r="B44" s="94"/>
+      <c r="C44" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="C39" s="23" t="s">
+      <c r="D44" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="D39" s="17"/>
-    </row>
-    <row r="40" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="32"/>
-      <c r="B40" s="30"/>
-      <c r="C40" s="22" t="s">
+      <c r="E44" s="20"/>
+    </row>
+    <row r="45" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="39"/>
+      <c r="B45" s="94"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="D40" s="17"/>
-    </row>
-    <row r="41" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="32"/>
-      <c r="B41" s="29" t="s">
+      <c r="E45" s="20"/>
+    </row>
+    <row r="46" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="39"/>
+      <c r="B46" s="94"/>
+      <c r="C46" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="C41" s="20" t="s">
+      <c r="D46" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="D41" s="17"/>
-    </row>
-    <row r="42" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="32"/>
-      <c r="B42" s="30"/>
-      <c r="C42" s="22" t="s">
+      <c r="E46" s="20"/>
+    </row>
+    <row r="47" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="39"/>
+      <c r="B47" s="94"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="D42" s="17"/>
-    </row>
-    <row r="43" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="32"/>
-      <c r="B43" s="30"/>
-      <c r="C43" s="22" t="s">
+      <c r="E47" s="20"/>
+    </row>
+    <row r="48" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="39"/>
+      <c r="B48" s="94"/>
+      <c r="C48" s="41"/>
+      <c r="D48" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="D43" s="17"/>
-    </row>
-    <row r="44" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="32"/>
-      <c r="B44" s="30"/>
-      <c r="C44" s="22" t="s">
+      <c r="E48" s="20"/>
+    </row>
+    <row r="49" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="39"/>
+      <c r="B49" s="94"/>
+      <c r="C49" s="41"/>
+      <c r="D49" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="D44" s="17"/>
-    </row>
-    <row r="45" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="32"/>
-      <c r="B45" s="30"/>
-      <c r="C45" s="22" t="s">
+      <c r="E49" s="20"/>
+    </row>
+    <row r="50" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="39"/>
+      <c r="B50" s="94"/>
+      <c r="C50" s="41"/>
+      <c r="D50" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="D45" s="17"/>
-    </row>
-    <row r="46" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="32"/>
-      <c r="B46" s="30"/>
-      <c r="C46" s="22" t="s">
+      <c r="E50" s="20"/>
+    </row>
+    <row r="51" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="39"/>
+      <c r="B51" s="95"/>
+      <c r="C51" s="41"/>
+      <c r="D51" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="D46" s="17"/>
-    </row>
-    <row r="47" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="33" t="s">
+      <c r="E51" s="20"/>
+    </row>
+    <row r="52" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="B52" s="70">
+        <v>2</v>
+      </c>
+      <c r="C52" s="71" t="s">
+        <v>66</v>
+      </c>
+      <c r="D52" s="72" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="50"/>
+      <c r="B53" s="73"/>
+      <c r="C53" s="72" t="s">
+        <v>50</v>
+      </c>
+      <c r="D53" s="72" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="B54" s="40">
+        <v>3</v>
+      </c>
+      <c r="C54" s="75" t="s">
+        <v>17</v>
+      </c>
+      <c r="D54" s="75" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="39"/>
+      <c r="B55" s="41"/>
+      <c r="C55" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="D55" s="74" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="39"/>
+      <c r="B56" s="41"/>
+      <c r="C56" s="41"/>
+      <c r="D56" s="74" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" s="96" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="66" t="s">
+        <v>136</v>
+      </c>
+      <c r="B57" s="82">
+        <v>1</v>
+      </c>
+      <c r="C57" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="D57" s="81" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="19" t="s">
+      <c r="B58" s="93">
+        <v>11</v>
+      </c>
+      <c r="C58" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="C47" s="21" t="s">
+      <c r="D58" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="D47" s="10"/>
-    </row>
-    <row r="48" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="34"/>
-      <c r="B48" s="21" t="s">
+      <c r="E58" s="10"/>
+    </row>
+    <row r="59" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="39"/>
+      <c r="B59" s="94"/>
+      <c r="C59" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="C48" s="21" t="s">
+      <c r="D59" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="D48" s="10"/>
-    </row>
-    <row r="49" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="34"/>
-      <c r="B49" s="35" t="s">
+      <c r="E59" s="10"/>
+    </row>
+    <row r="60" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="39"/>
+      <c r="B60" s="94"/>
+      <c r="C60" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="C49" s="21" t="s">
+      <c r="D60" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="D49" s="10"/>
-    </row>
-    <row r="50" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="34"/>
-      <c r="B50" s="36"/>
-      <c r="C50" s="21" t="s">
+      <c r="E60" s="10"/>
+    </row>
+    <row r="61" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="39"/>
+      <c r="B61" s="94"/>
+      <c r="C61" s="41"/>
+      <c r="D61" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="D50" s="10"/>
-    </row>
-    <row r="51" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="34"/>
-      <c r="B51" s="36"/>
-      <c r="C51" s="19" t="s">
+      <c r="E61" s="10"/>
+    </row>
+    <row r="62" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="39"/>
+      <c r="B62" s="94"/>
+      <c r="C62" s="41"/>
+      <c r="D62" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="D51" s="10"/>
-    </row>
-    <row r="52" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="34"/>
-      <c r="B52" s="36"/>
-      <c r="C52" s="19" t="s">
+      <c r="E62" s="10"/>
+    </row>
+    <row r="63" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="39"/>
+      <c r="B63" s="94"/>
+      <c r="C63" s="41"/>
+      <c r="D63" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="D52" s="10"/>
-    </row>
-    <row r="53" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="34"/>
-      <c r="B53" s="36"/>
-      <c r="C53" s="19" t="s">
+      <c r="E63" s="10"/>
+    </row>
+    <row r="64" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="39"/>
+      <c r="B64" s="94"/>
+      <c r="C64" s="41"/>
+      <c r="D64" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="D53" s="10"/>
-    </row>
-    <row r="54" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="34"/>
-      <c r="B54" s="19" t="s">
+      <c r="E64" s="10"/>
+    </row>
+    <row r="65" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="39"/>
+      <c r="B65" s="94"/>
+      <c r="C65" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="C54" s="21" t="s">
+      <c r="D65" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="D54" s="10"/>
-    </row>
-    <row r="55" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="34"/>
-      <c r="B55" s="35" t="s">
+      <c r="E65" s="10"/>
+    </row>
+    <row r="66" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="39"/>
+      <c r="B66" s="94"/>
+      <c r="C66" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="C55" s="21" t="s">
+      <c r="D66" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="D55" s="10"/>
-    </row>
-    <row r="56" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="34"/>
-      <c r="B56" s="36"/>
-      <c r="C56" s="19" t="s">
+      <c r="E66" s="10"/>
+    </row>
+    <row r="67" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="39"/>
+      <c r="B67" s="94"/>
+      <c r="C67" s="41"/>
+      <c r="D67" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="D56" s="10"/>
-    </row>
-    <row r="57" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="34"/>
-      <c r="B57" s="36"/>
-      <c r="C57" s="19" t="s">
+      <c r="E67" s="10"/>
+    </row>
+    <row r="68" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="39"/>
+      <c r="B68" s="94"/>
+      <c r="C68" s="41"/>
+      <c r="D68" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="D57" s="10"/>
-    </row>
-    <row r="58" spans="1:4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="34"/>
-      <c r="B58" s="36"/>
-      <c r="C58" s="19" t="s">
+      <c r="E68" s="10"/>
+    </row>
+    <row r="69" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="39"/>
+      <c r="B69" s="95"/>
+      <c r="C69" s="41"/>
+      <c r="D69" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="D58" s="10"/>
-    </row>
-    <row r="59" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D59" s="17"/>
-    </row>
-    <row r="60" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D60" s="17"/>
-    </row>
-    <row r="61" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D61" s="17"/>
-    </row>
-    <row r="62" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="15"/>
+      <c r="E69" s="10"/>
+    </row>
+    <row r="70" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="83" t="s">
+        <v>125</v>
+      </c>
+      <c r="B70" s="81">
+        <v>256</v>
+      </c>
+      <c r="C70" s="84" t="s">
+        <v>131</v>
+      </c>
+      <c r="D70" s="85"/>
+      <c r="E70" s="20"/>
+    </row>
+    <row r="71" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="B71" s="29">
+        <v>209</v>
+      </c>
+      <c r="C71" s="68" t="s">
+        <v>131</v>
+      </c>
+      <c r="D71" s="69"/>
+      <c r="E71" s="20"/>
+    </row>
+    <row r="72" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="83" t="s">
+        <v>127</v>
+      </c>
+      <c r="B72" s="81">
+        <v>136</v>
+      </c>
+      <c r="C72" s="84" t="s">
+        <v>131</v>
+      </c>
+      <c r="D72" s="85"/>
+      <c r="E72" s="20"/>
+    </row>
+    <row r="73" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="B73" s="29">
+        <v>24</v>
+      </c>
+      <c r="C73" s="68" t="s">
+        <v>131</v>
+      </c>
+      <c r="D73" s="69"/>
+    </row>
+    <row r="74" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="83" t="s">
+        <v>129</v>
+      </c>
+      <c r="B74" s="81">
+        <v>339</v>
+      </c>
+      <c r="C74" s="84" t="s">
+        <v>131</v>
+      </c>
+      <c r="D74" s="85"/>
+    </row>
+    <row r="75" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="B75" s="29">
+        <v>181</v>
+      </c>
+      <c r="C75" s="68" t="s">
+        <v>131</v>
+      </c>
+      <c r="D75" s="69"/>
+    </row>
+    <row r="76" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="67"/>
+      <c r="B76" s="67"/>
+      <c r="C76" s="67"/>
+      <c r="D76" s="86"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="32">
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C74:D74"/>
     <mergeCell ref="A5:A15"/>
-    <mergeCell ref="B9:B15"/>
+    <mergeCell ref="C9:C15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A19:A23"/>
-    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B19:B23"/>
+    <mergeCell ref="C24:C25"/>
     <mergeCell ref="A24:A26"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B30:B35"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B41:B46"/>
-    <mergeCell ref="A27:A46"/>
-    <mergeCell ref="A47:A58"/>
-    <mergeCell ref="B49:B53"/>
-    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C35:C40"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="B32:B51"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="C46:C51"/>
+    <mergeCell ref="A32:A51"/>
+    <mergeCell ref="A58:A69"/>
+    <mergeCell ref="C60:C64"/>
+    <mergeCell ref="C66:C69"/>
+    <mergeCell ref="B58:B69"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="B54:B56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1838,7 +2289,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1861,7 +2312,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="56" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1872,8 +2323,8 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="55"/>
-      <c r="B3" s="46" t="s">
+      <c r="A3" s="60"/>
+      <c r="B3" s="51" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1881,14 +2332,14 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="55"/>
-      <c r="B4" s="54"/>
+      <c r="A4" s="60"/>
+      <c r="B4" s="59"/>
       <c r="C4" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="55"/>
+      <c r="A5" s="60"/>
       <c r="B5" s="2" t="s">
         <v>59</v>
       </c>
@@ -1897,7 +2348,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="54"/>
+      <c r="A6" s="59"/>
       <c r="B6" s="2" t="s">
         <v>50</v>
       </c>
@@ -1906,10 +2357,10 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="57" t="s">
         <v>55</v>
       </c>
       <c r="C7" s="8" t="s">
@@ -1917,14 +2368,14 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="55"/>
-      <c r="B8" s="56"/>
+      <c r="A8" s="60"/>
+      <c r="B8" s="61"/>
       <c r="C8" s="8" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="54"/>
+      <c r="A9" s="59"/>
       <c r="B9" s="2" t="s">
         <v>56</v>
       </c>
@@ -1963,7 +2414,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1985,7 +2436,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="56" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -1996,7 +2447,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
+      <c r="A3" s="53"/>
       <c r="B3" s="2" t="s">
         <v>50</v>
       </c>
@@ -2026,7 +2477,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2048,7 +2499,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="54" t="s">
         <v>43</v>
       </c>
       <c r="B2" s="11" t="s">
@@ -2059,8 +2510,8 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="57"/>
-      <c r="B3" s="57" t="s">
+      <c r="A3" s="62"/>
+      <c r="B3" s="62" t="s">
         <v>50</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -2068,8 +2519,8 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="57"/>
-      <c r="B4" s="57"/>
+      <c r="A4" s="62"/>
+      <c r="B4" s="62"/>
       <c r="C4" s="8" t="s">
         <v>69</v>
       </c>
@@ -2091,7 +2542,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2138,161 +2589,161 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
+    <row r="2" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="26" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="58"/>
-      <c r="B3" s="29" t="s">
+    <row r="3" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="63"/>
+      <c r="B3" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="26" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="58"/>
-      <c r="B4" s="58"/>
-      <c r="C4" s="22" t="s">
+    <row r="4" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="63"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="25" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="58"/>
-      <c r="B5" s="29" t="s">
+    <row r="5" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="63"/>
+      <c r="B5" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="25" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="58"/>
-      <c r="B6" s="58"/>
-      <c r="C6" s="23" t="s">
+    <row r="6" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="63"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="26" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="58"/>
-      <c r="B7" s="58"/>
-      <c r="C7" s="22" t="s">
+    <row r="7" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="63"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="25" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="58"/>
-      <c r="B8" s="58"/>
-      <c r="C8" s="22" t="s">
+    <row r="8" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="63"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="25" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="58"/>
-      <c r="B9" s="58"/>
-      <c r="C9" s="22" t="s">
+    <row r="9" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="63"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="25" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="58"/>
-      <c r="B10" s="58"/>
-      <c r="C10" s="22" t="s">
+    <row r="10" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="63"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="25" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="58"/>
-      <c r="B11" s="22" t="s">
+    <row r="11" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="63"/>
+      <c r="B11" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="26" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="58"/>
-      <c r="B12" s="22" t="s">
+    <row r="12" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="63"/>
+      <c r="B12" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="26" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="58"/>
-      <c r="B13" s="22" t="s">
+    <row r="13" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="63"/>
+      <c r="B13" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="26" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="58"/>
-      <c r="B14" s="29" t="s">
+    <row r="14" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="63"/>
+      <c r="B14" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="26" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="58"/>
-      <c r="B15" s="58"/>
-      <c r="C15" s="22" t="s">
+    <row r="15" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="63"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="25" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="58"/>
-      <c r="B16" s="29" t="s">
+    <row r="16" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="63"/>
+      <c r="B16" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="27" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="58"/>
-      <c r="B17" s="58"/>
-      <c r="C17" s="22" t="s">
+    <row r="17" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="63"/>
+      <c r="B17" s="63"/>
+      <c r="C17" s="25" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="58"/>
-      <c r="B18" s="58"/>
-      <c r="C18" s="22" t="s">
+    <row r="18" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="63"/>
+      <c r="B18" s="63"/>
+      <c r="C18" s="25" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="58"/>
-      <c r="B19" s="58"/>
-      <c r="C19" s="22" t="s">
+    <row r="19" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="63"/>
+      <c r="B19" s="63"/>
+      <c r="C19" s="25" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="58"/>
-      <c r="B20" s="58"/>
-      <c r="C20" s="22" t="s">
+    <row r="20" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="63"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="25" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="58"/>
-      <c r="B21" s="58"/>
-      <c r="C21" s="22" t="s">
+    <row r="21" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="63"/>
+      <c r="B21" s="63"/>
+      <c r="C21" s="25" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2332,7 +2783,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="64" t="s">
         <v>46</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -2343,7 +2794,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="60"/>
+      <c r="A3" s="65"/>
       <c r="B3" t="s">
         <v>56</v>
       </c>
@@ -2352,8 +2803,8 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="60"/>
-      <c r="B4" s="59" t="s">
+      <c r="A4" s="65"/>
+      <c r="B4" s="64" t="s">
         <v>101</v>
       </c>
       <c r="C4" t="s">
@@ -2361,35 +2812,35 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="60"/>
-      <c r="B5" s="60"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="65"/>
       <c r="C5" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="60"/>
-      <c r="B6" s="60"/>
+      <c r="A6" s="65"/>
+      <c r="B6" s="65"/>
       <c r="C6" s="5" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="60"/>
-      <c r="B7" s="60"/>
+      <c r="A7" s="65"/>
+      <c r="B7" s="65"/>
       <c r="C7" s="5" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="60"/>
-      <c r="B8" s="60"/>
+      <c r="A8" s="65"/>
+      <c r="B8" s="65"/>
       <c r="C8" s="5" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="60"/>
+      <c r="A9" s="65"/>
       <c r="B9" s="5" t="s">
         <v>106</v>
       </c>
@@ -2398,8 +2849,8 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="60"/>
-      <c r="B10" s="59" t="s">
+      <c r="A10" s="65"/>
+      <c r="B10" s="64" t="s">
         <v>91</v>
       </c>
       <c r="C10" t="s">
@@ -2407,22 +2858,22 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="60"/>
-      <c r="B11" s="60"/>
+      <c r="A11" s="65"/>
+      <c r="B11" s="65"/>
       <c r="C11" s="5" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="60"/>
-      <c r="B12" s="60"/>
+      <c r="A12" s="65"/>
+      <c r="B12" s="65"/>
       <c r="C12" s="5" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="60"/>
-      <c r="B13" s="60"/>
+      <c r="A13" s="65"/>
+      <c r="B13" s="65"/>
       <c r="C13" s="5" t="s">
         <v>111</v>
       </c>
@@ -2600,7 +3051,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="51" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -2611,7 +3062,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="47"/>
+      <c r="A3" s="52"/>
       <c r="B3" s="8" t="s">
         <v>17</v>
       </c>
@@ -2620,7 +3071,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
+      <c r="A4" s="52"/>
       <c r="B4" s="8" t="s">
         <v>19</v>
       </c>
@@ -2629,7 +3080,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
+      <c r="A5" s="52"/>
       <c r="B5" s="8" t="s">
         <v>20</v>
       </c>
@@ -2638,8 +3089,8 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
-      <c r="B6" s="46" t="s">
+      <c r="A6" s="52"/>
+      <c r="B6" s="51" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -2647,43 +3098,43 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
-      <c r="B7" s="47"/>
+      <c r="A7" s="52"/>
+      <c r="B7" s="52"/>
       <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
-      <c r="B8" s="47"/>
+      <c r="A8" s="52"/>
+      <c r="B8" s="52"/>
       <c r="C8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
-      <c r="B9" s="47"/>
+      <c r="A9" s="52"/>
+      <c r="B9" s="52"/>
       <c r="C9" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
-      <c r="B10" s="47"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="52"/>
       <c r="C10" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
-      <c r="B11" s="47"/>
+      <c r="A11" s="52"/>
+      <c r="B11" s="52"/>
       <c r="C11" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="48"/>
-      <c r="B12" s="48"/>
+      <c r="A12" s="53"/>
+      <c r="B12" s="53"/>
       <c r="C12" s="2" t="s">
         <v>29</v>
       </c>
@@ -2727,7 +3178,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="54" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2738,7 +3189,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="50"/>
+      <c r="A3" s="55"/>
       <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
@@ -2841,7 +3292,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="56" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2852,7 +3303,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="47"/>
+      <c r="A3" s="52"/>
       <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
@@ -2861,7 +3312,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
+      <c r="A4" s="52"/>
       <c r="B4" s="2" t="s">
         <v>48</v>
       </c>
@@ -2870,7 +3321,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
+      <c r="A5" s="52"/>
       <c r="B5" s="2" t="s">
         <v>49</v>
       </c>
@@ -2879,7 +3330,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="48"/>
+      <c r="A6" s="53"/>
       <c r="B6" s="2" t="s">
         <v>50</v>
       </c>
@@ -2943,10 +3394,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="57" t="s">
         <v>55</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -2954,14 +3405,14 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="47"/>
-      <c r="B3" s="53"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="58"/>
       <c r="C3" s="8" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="48"/>
+      <c r="A4" s="53"/>
       <c r="B4" s="2" t="s">
         <v>56</v>
       </c>

</xml_diff>

<commit_message>
orthogrou species comparison files
</commit_message>
<xml_diff>
--- a/Output/SuppTables/Shared_GO.xlsx
+++ b/Output/SuppTables/Shared_GO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jillashey/Desktop/PutnamLab/Repositories/SedimentStress/SedimentStress/Output/SuppTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F598F43-07BA-B342-A9E1-83170C1132C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81670CB-F8FA-EC46-AAE9-81E2602A0C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16960" yWindow="660" windowWidth="18260" windowHeight="20360" xr2:uid="{463EAF44-39AF-B74B-A9CF-96AD4C6642C9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29080" windowHeight="20360" xr2:uid="{463EAF44-39AF-B74B-A9CF-96AD4C6642C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Full" sheetId="17" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="142">
   <si>
     <t>A.cervicornis + M.cavernosa + M.capitata</t>
   </si>
@@ -613,9 +613,6 @@
     <t xml:space="preserve">P.lobata </t>
   </si>
   <si>
-    <t>See Supplementary Table xx</t>
-  </si>
-  <si>
     <t>Number of shared GO terms</t>
   </si>
   <si>
@@ -629,6 +626,24 @@
   </si>
   <si>
     <t xml:space="preserve"> O.faveolata + P.acuta </t>
+  </si>
+  <si>
+    <t>See Supplementary Table S2</t>
+  </si>
+  <si>
+    <t>See Supplementary Table S5</t>
+  </si>
+  <si>
+    <t>See Supplementary Table S3</t>
+  </si>
+  <si>
+    <t>See Supplementary Table S4</t>
+  </si>
+  <si>
+    <t>See Supplementary Table S6</t>
+  </si>
+  <si>
+    <t>See Supplementary Table S7</t>
   </si>
 </sst>
 </file>
@@ -827,7 +842,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -871,9 +886,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -914,117 +926,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1035,19 +952,47 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1056,36 +1001,131 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1403,16 +1443,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{113029E7-F384-C24D-A58A-6D6AAA957483}">
   <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" zoomScale="91" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="91" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="45.5" style="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" style="20" customWidth="1"/>
-    <col min="3" max="3" width="35" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="112" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="112" style="105" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="10.83203125" style="17"/>
   </cols>
   <sheetData>
@@ -1421,832 +1461,848 @@
         <v>10</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="97" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="31"/>
+      <c r="E1" s="30"/>
     </row>
     <row r="2" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="B2" s="23">
+      <c r="B2" s="22">
         <v>1</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="98" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="20"/>
     </row>
     <row r="3" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="B3" s="34">
+      <c r="B3" s="33">
         <v>1</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="99" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="20"/>
     </row>
     <row r="4" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="B4" s="23">
+      <c r="B4" s="22">
         <v>1</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="98" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="20"/>
     </row>
     <row r="5" spans="1:5" s="18" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="62" t="s">
         <v>120</v>
       </c>
       <c r="B5" s="15"/>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="32"/>
+      <c r="E5" s="31"/>
     </row>
     <row r="6" spans="1:5" s="18" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
+      <c r="A6" s="63"/>
       <c r="B6" s="19"/>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="99" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="32"/>
+      <c r="E6" s="31"/>
     </row>
     <row r="7" spans="1:5" s="18" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
+      <c r="A7" s="63"/>
       <c r="B7" s="19"/>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="32"/>
+      <c r="E7" s="31"/>
     </row>
     <row r="8" spans="1:5" s="18" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
+      <c r="A8" s="63"/>
       <c r="B8" s="19"/>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="99" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="32"/>
+      <c r="E8" s="31"/>
     </row>
     <row r="9" spans="1:5" s="18" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
+      <c r="A9" s="63"/>
       <c r="B9" s="19"/>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="99" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="32"/>
+      <c r="E9" s="31"/>
     </row>
     <row r="10" spans="1:5" s="18" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
+      <c r="A10" s="63"/>
       <c r="B10" s="19">
         <v>11</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="28" t="s">
+      <c r="C10" s="63"/>
+      <c r="D10" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="32"/>
+      <c r="E10" s="31"/>
     </row>
     <row r="11" spans="1:5" s="18" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
+      <c r="A11" s="63"/>
       <c r="B11" s="19"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="28" t="s">
+      <c r="C11" s="63"/>
+      <c r="D11" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="32"/>
+      <c r="E11" s="31"/>
     </row>
     <row r="12" spans="1:5" s="18" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
+      <c r="A12" s="63"/>
       <c r="B12" s="19"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="28" t="s">
+      <c r="C12" s="63"/>
+      <c r="D12" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="31"/>
     </row>
     <row r="13" spans="1:5" s="18" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
+      <c r="A13" s="63"/>
       <c r="B13" s="19"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="28" t="s">
+      <c r="C13" s="63"/>
+      <c r="D13" s="99" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="32"/>
+      <c r="E13" s="31"/>
     </row>
     <row r="14" spans="1:5" s="18" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
+      <c r="A14" s="63"/>
       <c r="B14" s="19"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="28" t="s">
+      <c r="C14" s="63"/>
+      <c r="D14" s="99" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="32"/>
+      <c r="E14" s="31"/>
     </row>
     <row r="15" spans="1:5" s="18" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A15" s="43"/>
+      <c r="A15" s="64"/>
       <c r="B15" s="16"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="28" t="s">
+      <c r="C15" s="64"/>
+      <c r="D15" s="99" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="32"/>
+      <c r="E15" s="31"/>
     </row>
     <row r="16" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="70">
+      <c r="B16" s="67">
         <v>2</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="34" t="s">
         <v>51</v>
       </c>
       <c r="E16" s="20"/>
     </row>
     <row r="17" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="37"/>
-      <c r="B17" s="88"/>
-      <c r="C17" s="23" t="s">
+      <c r="A17" s="66"/>
+      <c r="B17" s="68"/>
+      <c r="C17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="34" t="s">
         <v>52</v>
       </c>
       <c r="E17" s="20"/>
     </row>
     <row r="18" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="B18" s="29">
+      <c r="B18" s="28">
         <v>1</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="22" t="s">
+      <c r="D18" s="100" t="s">
         <v>54</v>
       </c>
       <c r="E18" s="20"/>
     </row>
     <row r="19" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="B19" s="70">
+      <c r="B19" s="67">
         <v>5</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="34" t="s">
         <v>112</v>
       </c>
       <c r="E19" s="20"/>
     </row>
     <row r="20" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="49"/>
-      <c r="B20" s="89"/>
-      <c r="C20" s="23" t="s">
+      <c r="A20" s="56"/>
+      <c r="B20" s="69"/>
+      <c r="C20" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="34" t="s">
         <v>113</v>
       </c>
       <c r="E20" s="20"/>
     </row>
     <row r="21" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="49"/>
-      <c r="B21" s="89"/>
-      <c r="C21" s="23" t="s">
+      <c r="A21" s="56"/>
+      <c r="B21" s="69"/>
+      <c r="C21" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="D21" s="34" t="s">
         <v>114</v>
       </c>
       <c r="E21" s="20"/>
     </row>
     <row r="22" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="49"/>
-      <c r="B22" s="89"/>
-      <c r="C22" s="23" t="s">
+      <c r="A22" s="56"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="34" t="s">
         <v>115</v>
       </c>
       <c r="E22" s="20"/>
     </row>
     <row r="23" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="50"/>
-      <c r="B23" s="88"/>
-      <c r="C23" s="23" t="s">
+      <c r="A23" s="57"/>
+      <c r="B23" s="68"/>
+      <c r="C23" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="25" t="s">
+      <c r="D23" s="34" t="s">
         <v>116</v>
       </c>
       <c r="E23" s="20"/>
     </row>
     <row r="24" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="44" t="s">
+      <c r="A24" s="70" t="s">
         <v>123</v>
       </c>
-      <c r="B24" s="90"/>
-      <c r="C24" s="42" t="s">
+      <c r="B24" s="49"/>
+      <c r="C24" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="22" t="s">
+      <c r="D24" s="100" t="s">
         <v>57</v>
       </c>
       <c r="E24" s="20"/>
     </row>
-    <row r="25" spans="1:5" s="76" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="45"/>
-      <c r="B25" s="91">
+    <row r="25" spans="1:5" s="42" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="71"/>
+      <c r="B25" s="50">
         <v>3</v>
       </c>
-      <c r="C25" s="43"/>
-      <c r="D25" s="77" t="s">
+      <c r="C25" s="64"/>
+      <c r="D25" s="40" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="76" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="46"/>
-      <c r="B26" s="92"/>
-      <c r="C26" s="78" t="s">
+    <row r="26" spans="1:5" s="42" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="72"/>
+      <c r="B26" s="51"/>
+      <c r="C26" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="77" t="s">
+      <c r="D26" s="40" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="76" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="48" t="s">
+    <row r="27" spans="1:5" s="42" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="55" t="s">
+        <v>132</v>
+      </c>
+      <c r="B27" s="67">
+        <v>4</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="42" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="56"/>
+      <c r="B28" s="78"/>
+      <c r="C28" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="42" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="56"/>
+      <c r="B29" s="78"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="35" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="42" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="56"/>
+      <c r="B30" s="78"/>
+      <c r="C30" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="35" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="42" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="57"/>
+      <c r="B31" s="59"/>
+      <c r="C31" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="35" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="42" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="79" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="75">
+        <v>20</v>
+      </c>
+      <c r="C32" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="D32" s="48" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="42" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="80"/>
+      <c r="B33" s="76"/>
+      <c r="C33" s="73" t="s">
+        <v>73</v>
+      </c>
+      <c r="D33" s="48" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="80"/>
+      <c r="B34" s="76"/>
+      <c r="C34" s="74"/>
+      <c r="D34" s="100" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" s="20"/>
+    </row>
+    <row r="35" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="80"/>
+      <c r="B35" s="76"/>
+      <c r="C35" s="73" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" s="100" t="s">
+        <v>79</v>
+      </c>
+      <c r="E35" s="20"/>
+    </row>
+    <row r="36" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="80"/>
+      <c r="B36" s="76"/>
+      <c r="C36" s="74"/>
+      <c r="D36" s="99" t="s">
+        <v>80</v>
+      </c>
+      <c r="E36" s="20"/>
+    </row>
+    <row r="37" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="80"/>
+      <c r="B37" s="76"/>
+      <c r="C37" s="74"/>
+      <c r="D37" s="100" t="s">
+        <v>81</v>
+      </c>
+      <c r="E37" s="20"/>
+    </row>
+    <row r="38" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="80"/>
+      <c r="B38" s="76"/>
+      <c r="C38" s="74"/>
+      <c r="D38" s="100" t="s">
+        <v>82</v>
+      </c>
+      <c r="E38" s="20"/>
+    </row>
+    <row r="39" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="80"/>
+      <c r="B39" s="76"/>
+      <c r="C39" s="74"/>
+      <c r="D39" s="100" t="s">
+        <v>83</v>
+      </c>
+      <c r="E39" s="20"/>
+    </row>
+    <row r="40" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="80"/>
+      <c r="B40" s="76"/>
+      <c r="C40" s="74"/>
+      <c r="D40" s="100" t="s">
+        <v>84</v>
+      </c>
+      <c r="E40" s="20"/>
+    </row>
+    <row r="41" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="80"/>
+      <c r="B41" s="76"/>
+      <c r="C41" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" s="99" t="s">
+        <v>85</v>
+      </c>
+      <c r="E41" s="20"/>
+    </row>
+    <row r="42" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="80"/>
+      <c r="B42" s="76"/>
+      <c r="C42" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42" s="99" t="s">
+        <v>71</v>
+      </c>
+      <c r="E42" s="20"/>
+    </row>
+    <row r="43" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="80"/>
+      <c r="B43" s="76"/>
+      <c r="C43" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="D43" s="99" t="s">
+        <v>87</v>
+      </c>
+      <c r="E43" s="20"/>
+    </row>
+    <row r="44" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="80"/>
+      <c r="B44" s="76"/>
+      <c r="C44" s="73" t="s">
+        <v>88</v>
+      </c>
+      <c r="D44" s="99" t="s">
+        <v>89</v>
+      </c>
+      <c r="E44" s="20"/>
+    </row>
+    <row r="45" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="80"/>
+      <c r="B45" s="76"/>
+      <c r="C45" s="74"/>
+      <c r="D45" s="100" t="s">
+        <v>90</v>
+      </c>
+      <c r="E45" s="20"/>
+    </row>
+    <row r="46" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="80"/>
+      <c r="B46" s="76"/>
+      <c r="C46" s="73" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" s="101" t="s">
+        <v>92</v>
+      </c>
+      <c r="E46" s="20"/>
+    </row>
+    <row r="47" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="80"/>
+      <c r="B47" s="76"/>
+      <c r="C47" s="74"/>
+      <c r="D47" s="100" t="s">
+        <v>93</v>
+      </c>
+      <c r="E47" s="20"/>
+    </row>
+    <row r="48" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="80"/>
+      <c r="B48" s="76"/>
+      <c r="C48" s="74"/>
+      <c r="D48" s="100" t="s">
+        <v>94</v>
+      </c>
+      <c r="E48" s="20"/>
+    </row>
+    <row r="49" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="80"/>
+      <c r="B49" s="76"/>
+      <c r="C49" s="74"/>
+      <c r="D49" s="100" t="s">
+        <v>95</v>
+      </c>
+      <c r="E49" s="20"/>
+    </row>
+    <row r="50" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="80"/>
+      <c r="B50" s="76"/>
+      <c r="C50" s="74"/>
+      <c r="D50" s="100" t="s">
+        <v>96</v>
+      </c>
+      <c r="E50" s="20"/>
+    </row>
+    <row r="51" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="80"/>
+      <c r="B51" s="77"/>
+      <c r="C51" s="74"/>
+      <c r="D51" s="100" t="s">
+        <v>97</v>
+      </c>
+      <c r="E51" s="20"/>
+    </row>
+    <row r="52" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="55" t="s">
         <v>133</v>
       </c>
-      <c r="B27" s="70">
-        <v>4</v>
-      </c>
-      <c r="C27" s="23" t="s">
+      <c r="B52" s="67">
+        <v>2</v>
+      </c>
+      <c r="C52" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="D52" s="102" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="57"/>
+      <c r="B53" s="59"/>
+      <c r="C53" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" s="102" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="79" t="s">
+        <v>134</v>
+      </c>
+      <c r="B54" s="73">
+        <v>3</v>
+      </c>
+      <c r="C54" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D54" s="44" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="80"/>
+      <c r="B55" s="74"/>
+      <c r="C55" s="74" t="s">
+        <v>18</v>
+      </c>
+      <c r="D55" s="43" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="80"/>
+      <c r="B56" s="74"/>
+      <c r="C56" s="74"/>
+      <c r="D56" s="43" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" s="52" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="B57" s="46">
+        <v>1</v>
+      </c>
+      <c r="C57" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="D57" s="103" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="79" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" s="75">
+        <v>11</v>
+      </c>
+      <c r="C58" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="D58" s="101" t="s">
+        <v>99</v>
+      </c>
+      <c r="E58" s="10"/>
+    </row>
+    <row r="59" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="80"/>
+      <c r="B59" s="76"/>
+      <c r="C59" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="D27" s="23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" s="76" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="49"/>
-      <c r="B28" s="79"/>
-      <c r="C28" s="80" t="s">
-        <v>17</v>
-      </c>
-      <c r="D28" s="23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" s="76" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="49"/>
-      <c r="B29" s="79"/>
-      <c r="C29" s="73"/>
-      <c r="D29" s="23" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" s="76" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="49"/>
-      <c r="B30" s="79"/>
-      <c r="C30" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="D30" s="23" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" s="76" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="50"/>
-      <c r="B31" s="73"/>
-      <c r="C31" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D31" s="23" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" s="76" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" s="93">
-        <v>20</v>
-      </c>
-      <c r="C32" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="D32" s="87" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="76" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="39"/>
-      <c r="B33" s="94"/>
-      <c r="C33" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="D33" s="87" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="39"/>
-      <c r="B34" s="94"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="E34" s="20"/>
-    </row>
-    <row r="35" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="39"/>
-      <c r="B35" s="94"/>
-      <c r="C35" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="D35" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="E35" s="20"/>
-    </row>
-    <row r="36" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="39"/>
-      <c r="B36" s="94"/>
-      <c r="C36" s="41"/>
-      <c r="D36" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="E36" s="20"/>
-    </row>
-    <row r="37" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="39"/>
-      <c r="B37" s="94"/>
-      <c r="C37" s="41"/>
-      <c r="D37" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="E37" s="20"/>
-    </row>
-    <row r="38" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="39"/>
-      <c r="B38" s="94"/>
-      <c r="C38" s="41"/>
-      <c r="D38" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="E38" s="20"/>
-    </row>
-    <row r="39" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="39"/>
-      <c r="B39" s="94"/>
-      <c r="C39" s="41"/>
-      <c r="D39" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="E39" s="20"/>
-    </row>
-    <row r="40" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="39"/>
-      <c r="B40" s="94"/>
-      <c r="C40" s="41"/>
-      <c r="D40" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="E40" s="20"/>
-    </row>
-    <row r="41" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="39"/>
-      <c r="B41" s="94"/>
-      <c r="C41" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="D41" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="E41" s="20"/>
-    </row>
-    <row r="42" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="39"/>
-      <c r="B42" s="94"/>
-      <c r="C42" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="D42" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="E42" s="20"/>
-    </row>
-    <row r="43" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="39"/>
-      <c r="B43" s="94"/>
-      <c r="C43" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="D43" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="E43" s="20"/>
-    </row>
-    <row r="44" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="39"/>
-      <c r="B44" s="94"/>
-      <c r="C44" s="40" t="s">
-        <v>88</v>
-      </c>
-      <c r="D44" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="E44" s="20"/>
-    </row>
-    <row r="45" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="39"/>
-      <c r="B45" s="94"/>
-      <c r="C45" s="41"/>
-      <c r="D45" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="E45" s="20"/>
-    </row>
-    <row r="46" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="39"/>
-      <c r="B46" s="94"/>
-      <c r="C46" s="40" t="s">
+      <c r="D59" s="101" t="s">
+        <v>100</v>
+      </c>
+      <c r="E59" s="10"/>
+    </row>
+    <row r="60" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="80"/>
+      <c r="B60" s="76"/>
+      <c r="C60" s="73" t="s">
+        <v>101</v>
+      </c>
+      <c r="D60" s="101" t="s">
+        <v>102</v>
+      </c>
+      <c r="E60" s="10"/>
+    </row>
+    <row r="61" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="80"/>
+      <c r="B61" s="76"/>
+      <c r="C61" s="74"/>
+      <c r="D61" s="101" t="s">
+        <v>103</v>
+      </c>
+      <c r="E61" s="10"/>
+    </row>
+    <row r="62" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="80"/>
+      <c r="B62" s="76"/>
+      <c r="C62" s="74"/>
+      <c r="D62" s="100" t="s">
+        <v>104</v>
+      </c>
+      <c r="E62" s="10"/>
+    </row>
+    <row r="63" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="80"/>
+      <c r="B63" s="76"/>
+      <c r="C63" s="74"/>
+      <c r="D63" s="100" t="s">
+        <v>100</v>
+      </c>
+      <c r="E63" s="10"/>
+    </row>
+    <row r="64" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="80"/>
+      <c r="B64" s="76"/>
+      <c r="C64" s="74"/>
+      <c r="D64" s="100" t="s">
+        <v>105</v>
+      </c>
+      <c r="E64" s="10"/>
+    </row>
+    <row r="65" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="80"/>
+      <c r="B65" s="76"/>
+      <c r="C65" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="D65" s="101" t="s">
+        <v>107</v>
+      </c>
+      <c r="E65" s="10"/>
+    </row>
+    <row r="66" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="80"/>
+      <c r="B66" s="76"/>
+      <c r="C66" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="D46" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="E46" s="20"/>
-    </row>
-    <row r="47" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="39"/>
-      <c r="B47" s="94"/>
-      <c r="C47" s="41"/>
-      <c r="D47" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="E47" s="20"/>
-    </row>
-    <row r="48" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="39"/>
-      <c r="B48" s="94"/>
-      <c r="C48" s="41"/>
-      <c r="D48" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="E48" s="20"/>
-    </row>
-    <row r="49" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="39"/>
-      <c r="B49" s="94"/>
-      <c r="C49" s="41"/>
-      <c r="D49" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="E49" s="20"/>
-    </row>
-    <row r="50" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="39"/>
-      <c r="B50" s="94"/>
-      <c r="C50" s="41"/>
-      <c r="D50" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="E50" s="20"/>
-    </row>
-    <row r="51" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="39"/>
-      <c r="B51" s="95"/>
-      <c r="C51" s="41"/>
-      <c r="D51" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="E51" s="20"/>
-    </row>
-    <row r="52" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="48" t="s">
-        <v>134</v>
-      </c>
-      <c r="B52" s="70">
-        <v>2</v>
-      </c>
-      <c r="C52" s="71" t="s">
-        <v>66</v>
-      </c>
-      <c r="D52" s="72" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="50"/>
-      <c r="B53" s="73"/>
-      <c r="C53" s="72" t="s">
-        <v>50</v>
-      </c>
-      <c r="D53" s="72" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="38" t="s">
-        <v>135</v>
-      </c>
-      <c r="B54" s="40">
-        <v>3</v>
-      </c>
-      <c r="C54" s="75" t="s">
-        <v>17</v>
-      </c>
-      <c r="D54" s="75" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="39"/>
-      <c r="B55" s="41"/>
-      <c r="C55" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="D55" s="74" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="39"/>
-      <c r="B56" s="41"/>
-      <c r="C56" s="41"/>
-      <c r="D56" s="74" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" s="96" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="66" t="s">
+      <c r="D66" s="101" t="s">
+        <v>108</v>
+      </c>
+      <c r="E66" s="10"/>
+    </row>
+    <row r="67" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="80"/>
+      <c r="B67" s="76"/>
+      <c r="C67" s="74"/>
+      <c r="D67" s="100" t="s">
+        <v>109</v>
+      </c>
+      <c r="E67" s="10"/>
+    </row>
+    <row r="68" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="80"/>
+      <c r="B68" s="76"/>
+      <c r="C68" s="74"/>
+      <c r="D68" s="100" t="s">
+        <v>110</v>
+      </c>
+      <c r="E68" s="10"/>
+    </row>
+    <row r="69" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="80"/>
+      <c r="B69" s="77"/>
+      <c r="C69" s="74"/>
+      <c r="D69" s="100" t="s">
+        <v>111</v>
+      </c>
+      <c r="E69" s="10"/>
+    </row>
+    <row r="70" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="47" t="s">
+        <v>125</v>
+      </c>
+      <c r="B70" s="45">
+        <v>256</v>
+      </c>
+      <c r="C70" s="60" t="s">
         <v>136</v>
       </c>
-      <c r="B57" s="82">
-        <v>1</v>
-      </c>
-      <c r="C57" s="82" t="s">
-        <v>47</v>
-      </c>
-      <c r="D57" s="81" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="B58" s="93">
-        <v>11</v>
-      </c>
-      <c r="C58" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="D58" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="E58" s="10"/>
-    </row>
-    <row r="59" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="39"/>
-      <c r="B59" s="94"/>
-      <c r="C59" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="D59" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="E59" s="10"/>
-    </row>
-    <row r="60" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="39"/>
-      <c r="B60" s="94"/>
-      <c r="C60" s="40" t="s">
-        <v>101</v>
-      </c>
-      <c r="D60" s="34" t="s">
-        <v>102</v>
-      </c>
-      <c r="E60" s="10"/>
-    </row>
-    <row r="61" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="39"/>
-      <c r="B61" s="94"/>
-      <c r="C61" s="41"/>
-      <c r="D61" s="34" t="s">
-        <v>103</v>
-      </c>
-      <c r="E61" s="10"/>
-    </row>
-    <row r="62" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="39"/>
-      <c r="B62" s="94"/>
-      <c r="C62" s="41"/>
-      <c r="D62" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="E62" s="10"/>
-    </row>
-    <row r="63" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="39"/>
-      <c r="B63" s="94"/>
-      <c r="C63" s="41"/>
-      <c r="D63" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="E63" s="10"/>
-    </row>
-    <row r="64" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="39"/>
-      <c r="B64" s="94"/>
-      <c r="C64" s="41"/>
-      <c r="D64" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="E64" s="10"/>
-    </row>
-    <row r="65" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="39"/>
-      <c r="B65" s="94"/>
-      <c r="C65" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="D65" s="34" t="s">
-        <v>107</v>
-      </c>
-      <c r="E65" s="10"/>
-    </row>
-    <row r="66" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="39"/>
-      <c r="B66" s="94"/>
-      <c r="C66" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="D66" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="E66" s="10"/>
-    </row>
-    <row r="67" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="39"/>
-      <c r="B67" s="94"/>
-      <c r="C67" s="41"/>
-      <c r="D67" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="E67" s="10"/>
-    </row>
-    <row r="68" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="39"/>
-      <c r="B68" s="94"/>
-      <c r="C68" s="41"/>
-      <c r="D68" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="E68" s="10"/>
-    </row>
-    <row r="69" spans="1:5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="39"/>
-      <c r="B69" s="95"/>
-      <c r="C69" s="41"/>
-      <c r="D69" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="E69" s="10"/>
-    </row>
-    <row r="70" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="83" t="s">
-        <v>125</v>
-      </c>
-      <c r="B70" s="81">
-        <v>256</v>
-      </c>
-      <c r="C70" s="84" t="s">
-        <v>131</v>
-      </c>
-      <c r="D70" s="85"/>
+      <c r="D70" s="61"/>
       <c r="E70" s="20"/>
     </row>
     <row r="71" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="33" t="s">
+      <c r="A71" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="B71" s="29">
+      <c r="B71" s="28">
         <v>209</v>
       </c>
-      <c r="C71" s="68" t="s">
-        <v>131</v>
-      </c>
-      <c r="D71" s="69"/>
+      <c r="C71" s="53" t="s">
+        <v>137</v>
+      </c>
+      <c r="D71" s="54"/>
       <c r="E71" s="20"/>
     </row>
     <row r="72" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="83" t="s">
+      <c r="A72" s="47" t="s">
         <v>127</v>
       </c>
-      <c r="B72" s="81">
+      <c r="B72" s="45">
         <v>136</v>
       </c>
-      <c r="C72" s="84" t="s">
-        <v>131</v>
-      </c>
-      <c r="D72" s="85"/>
+      <c r="C72" s="60" t="s">
+        <v>138</v>
+      </c>
+      <c r="D72" s="61"/>
       <c r="E72" s="20"/>
     </row>
     <row r="73" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="33" t="s">
+      <c r="A73" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="B73" s="29">
+      <c r="B73" s="28">
         <v>24</v>
       </c>
-      <c r="C73" s="68" t="s">
-        <v>131</v>
-      </c>
-      <c r="D73" s="69"/>
+      <c r="C73" s="53" t="s">
+        <v>139</v>
+      </c>
+      <c r="D73" s="54"/>
     </row>
     <row r="74" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="83" t="s">
+      <c r="A74" s="47" t="s">
         <v>129</v>
       </c>
-      <c r="B74" s="81">
+      <c r="B74" s="45">
         <v>339</v>
       </c>
-      <c r="C74" s="84" t="s">
-        <v>131</v>
-      </c>
-      <c r="D74" s="85"/>
+      <c r="C74" s="60" t="s">
+        <v>140</v>
+      </c>
+      <c r="D74" s="61"/>
     </row>
     <row r="75" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="33" t="s">
+      <c r="A75" s="32" t="s">
         <v>130</v>
       </c>
-      <c r="B75" s="29">
+      <c r="B75" s="28">
         <v>181</v>
       </c>
-      <c r="C75" s="68" t="s">
-        <v>131</v>
-      </c>
-      <c r="D75" s="69"/>
+      <c r="C75" s="53" t="s">
+        <v>141</v>
+      </c>
+      <c r="D75" s="54"/>
     </row>
     <row r="76" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="67"/>
-      <c r="B76" s="67"/>
-      <c r="C76" s="67"/>
-      <c r="D76" s="86"/>
+      <c r="A76" s="37"/>
+      <c r="B76" s="37"/>
+      <c r="C76" s="37"/>
+      <c r="D76" s="104"/>
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C35:C40"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="B32:B51"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="C46:C51"/>
+    <mergeCell ref="A32:A51"/>
+    <mergeCell ref="A5:A15"/>
+    <mergeCell ref="C9:C15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B19:B23"/>
     <mergeCell ref="C75:D75"/>
     <mergeCell ref="A27:A31"/>
     <mergeCell ref="C28:C29"/>
@@ -2256,21 +2312,6 @@
     <mergeCell ref="C72:D72"/>
     <mergeCell ref="C73:D73"/>
     <mergeCell ref="C74:D74"/>
-    <mergeCell ref="A5:A15"/>
-    <mergeCell ref="C9:C15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A19:A23"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B19:B23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C35:C40"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="B32:B51"/>
-    <mergeCell ref="B27:B31"/>
-    <mergeCell ref="C46:C51"/>
-    <mergeCell ref="A32:A51"/>
     <mergeCell ref="A58:A69"/>
     <mergeCell ref="C60:C64"/>
     <mergeCell ref="C66:C69"/>
@@ -2278,7 +2319,6 @@
     <mergeCell ref="A54:A56"/>
     <mergeCell ref="C55:C56"/>
     <mergeCell ref="B52:B53"/>
-    <mergeCell ref="B54:B56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2312,7 +2352,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="86" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2323,8 +2363,8 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="60"/>
-      <c r="B3" s="51" t="s">
+      <c r="A3" s="90"/>
+      <c r="B3" s="81" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -2332,14 +2372,14 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="60"/>
-      <c r="B4" s="59"/>
+      <c r="A4" s="90"/>
+      <c r="B4" s="89"/>
       <c r="C4" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="60"/>
+      <c r="A5" s="90"/>
       <c r="B5" s="2" t="s">
         <v>59</v>
       </c>
@@ -2348,7 +2388,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="59"/>
+      <c r="A6" s="89"/>
       <c r="B6" s="2" t="s">
         <v>50</v>
       </c>
@@ -2357,10 +2397,10 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="86" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="87" t="s">
         <v>55</v>
       </c>
       <c r="C7" s="8" t="s">
@@ -2368,14 +2408,14 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="60"/>
-      <c r="B8" s="61"/>
+      <c r="A8" s="90"/>
+      <c r="B8" s="91"/>
       <c r="C8" s="8" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="59"/>
+      <c r="A9" s="89"/>
       <c r="B9" s="2" t="s">
         <v>56</v>
       </c>
@@ -2436,7 +2476,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="86" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -2447,7 +2487,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="53"/>
+      <c r="A3" s="83"/>
       <c r="B3" s="2" t="s">
         <v>50</v>
       </c>
@@ -2499,7 +2539,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="84" t="s">
         <v>43</v>
       </c>
       <c r="B2" s="11" t="s">
@@ -2510,8 +2550,8 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="62"/>
-      <c r="B3" s="62" t="s">
+      <c r="A3" s="92"/>
+      <c r="B3" s="92" t="s">
         <v>50</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -2519,8 +2559,8 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="62"/>
-      <c r="B4" s="62"/>
+      <c r="A4" s="92"/>
+      <c r="B4" s="92"/>
       <c r="C4" s="8" t="s">
         <v>69</v>
       </c>
@@ -2590,160 +2630,160 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="2" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="93" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="25" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="63"/>
-      <c r="B3" s="35" t="s">
+      <c r="A3" s="94"/>
+      <c r="B3" s="93" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="25" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="63"/>
-      <c r="B4" s="63"/>
-      <c r="C4" s="25" t="s">
+      <c r="A4" s="94"/>
+      <c r="B4" s="94"/>
+      <c r="C4" s="24" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="63"/>
-      <c r="B5" s="35" t="s">
+      <c r="A5" s="94"/>
+      <c r="B5" s="93" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="24" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="63"/>
-      <c r="B6" s="63"/>
-      <c r="C6" s="26" t="s">
+      <c r="A6" s="94"/>
+      <c r="B6" s="94"/>
+      <c r="C6" s="25" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="63"/>
-      <c r="B7" s="63"/>
-      <c r="C7" s="25" t="s">
+      <c r="A7" s="94"/>
+      <c r="B7" s="94"/>
+      <c r="C7" s="24" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="63"/>
-      <c r="B8" s="63"/>
-      <c r="C8" s="25" t="s">
+      <c r="A8" s="94"/>
+      <c r="B8" s="94"/>
+      <c r="C8" s="24" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="63"/>
-      <c r="B9" s="63"/>
-      <c r="C9" s="25" t="s">
+      <c r="A9" s="94"/>
+      <c r="B9" s="94"/>
+      <c r="C9" s="24" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="63"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="25" t="s">
+      <c r="A10" s="94"/>
+      <c r="B10" s="94"/>
+      <c r="C10" s="24" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="63"/>
-      <c r="B11" s="25" t="s">
+      <c r="A11" s="94"/>
+      <c r="B11" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="25" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="63"/>
-      <c r="B12" s="25" t="s">
+      <c r="A12" s="94"/>
+      <c r="B12" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="25" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="63"/>
-      <c r="B13" s="25" t="s">
+      <c r="A13" s="94"/>
+      <c r="B13" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="25" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="63"/>
-      <c r="B14" s="35" t="s">
+      <c r="A14" s="94"/>
+      <c r="B14" s="93" t="s">
         <v>88</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="25" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="63"/>
-      <c r="B15" s="63"/>
-      <c r="C15" s="25" t="s">
+      <c r="A15" s="94"/>
+      <c r="B15" s="94"/>
+      <c r="C15" s="24" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="63"/>
-      <c r="B16" s="35" t="s">
+      <c r="A16" s="94"/>
+      <c r="B16" s="93" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="26" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="63"/>
-      <c r="B17" s="63"/>
-      <c r="C17" s="25" t="s">
+      <c r="A17" s="94"/>
+      <c r="B17" s="94"/>
+      <c r="C17" s="24" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="63"/>
-      <c r="B18" s="63"/>
-      <c r="C18" s="25" t="s">
+      <c r="A18" s="94"/>
+      <c r="B18" s="94"/>
+      <c r="C18" s="24" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="63"/>
-      <c r="B19" s="63"/>
-      <c r="C19" s="25" t="s">
+      <c r="A19" s="94"/>
+      <c r="B19" s="94"/>
+      <c r="C19" s="24" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="63"/>
-      <c r="B20" s="63"/>
-      <c r="C20" s="25" t="s">
+      <c r="A20" s="94"/>
+      <c r="B20" s="94"/>
+      <c r="C20" s="24" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="63"/>
-      <c r="B21" s="63"/>
-      <c r="C21" s="25" t="s">
+      <c r="A21" s="94"/>
+      <c r="B21" s="94"/>
+      <c r="C21" s="24" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2783,7 +2823,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="95" t="s">
         <v>46</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -2794,7 +2834,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="65"/>
+      <c r="A3" s="96"/>
       <c r="B3" t="s">
         <v>56</v>
       </c>
@@ -2803,8 +2843,8 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="65"/>
-      <c r="B4" s="64" t="s">
+      <c r="A4" s="96"/>
+      <c r="B4" s="95" t="s">
         <v>101</v>
       </c>
       <c r="C4" t="s">
@@ -2812,35 +2852,35 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="65"/>
-      <c r="B5" s="65"/>
+      <c r="A5" s="96"/>
+      <c r="B5" s="96"/>
       <c r="C5" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="65"/>
-      <c r="B6" s="65"/>
+      <c r="A6" s="96"/>
+      <c r="B6" s="96"/>
       <c r="C6" s="5" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="65"/>
-      <c r="B7" s="65"/>
+      <c r="A7" s="96"/>
+      <c r="B7" s="96"/>
       <c r="C7" s="5" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="65"/>
-      <c r="B8" s="65"/>
+      <c r="A8" s="96"/>
+      <c r="B8" s="96"/>
       <c r="C8" s="5" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="65"/>
+      <c r="A9" s="96"/>
       <c r="B9" s="5" t="s">
         <v>106</v>
       </c>
@@ -2849,8 +2889,8 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="65"/>
-      <c r="B10" s="64" t="s">
+      <c r="A10" s="96"/>
+      <c r="B10" s="95" t="s">
         <v>91</v>
       </c>
       <c r="C10" t="s">
@@ -2858,22 +2898,22 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="65"/>
-      <c r="B11" s="65"/>
+      <c r="A11" s="96"/>
+      <c r="B11" s="96"/>
       <c r="C11" s="5" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="65"/>
-      <c r="B12" s="65"/>
+      <c r="A12" s="96"/>
+      <c r="B12" s="96"/>
       <c r="C12" s="5" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="65"/>
-      <c r="B13" s="65"/>
+      <c r="A13" s="96"/>
+      <c r="B13" s="96"/>
       <c r="C13" s="5" t="s">
         <v>111</v>
       </c>
@@ -3051,7 +3091,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="81" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -3062,7 +3102,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="52"/>
+      <c r="A3" s="82"/>
       <c r="B3" s="8" t="s">
         <v>17</v>
       </c>
@@ -3071,7 +3111,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="52"/>
+      <c r="A4" s="82"/>
       <c r="B4" s="8" t="s">
         <v>19</v>
       </c>
@@ -3080,7 +3120,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="52"/>
+      <c r="A5" s="82"/>
       <c r="B5" s="8" t="s">
         <v>20</v>
       </c>
@@ -3089,8 +3129,8 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="52"/>
-      <c r="B6" s="51" t="s">
+      <c r="A6" s="82"/>
+      <c r="B6" s="81" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -3098,43 +3138,43 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="52"/>
-      <c r="B7" s="52"/>
+      <c r="A7" s="82"/>
+      <c r="B7" s="82"/>
       <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="52"/>
-      <c r="B8" s="52"/>
+      <c r="A8" s="82"/>
+      <c r="B8" s="82"/>
       <c r="C8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="52"/>
-      <c r="B9" s="52"/>
+      <c r="A9" s="82"/>
+      <c r="B9" s="82"/>
       <c r="C9" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="52"/>
-      <c r="B10" s="52"/>
+      <c r="A10" s="82"/>
+      <c r="B10" s="82"/>
       <c r="C10" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="52"/>
-      <c r="B11" s="52"/>
+      <c r="A11" s="82"/>
+      <c r="B11" s="82"/>
       <c r="C11" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="53"/>
-      <c r="B12" s="53"/>
+      <c r="A12" s="83"/>
+      <c r="B12" s="83"/>
       <c r="C12" s="2" t="s">
         <v>29</v>
       </c>
@@ -3178,7 +3218,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="84" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -3189,7 +3229,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="55"/>
+      <c r="A3" s="85"/>
       <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
@@ -3292,7 +3332,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="86" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -3303,7 +3343,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="52"/>
+      <c r="A3" s="82"/>
       <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
@@ -3312,7 +3352,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="52"/>
+      <c r="A4" s="82"/>
       <c r="B4" s="2" t="s">
         <v>48</v>
       </c>
@@ -3321,7 +3361,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="52"/>
+      <c r="A5" s="82"/>
       <c r="B5" s="2" t="s">
         <v>49</v>
       </c>
@@ -3330,7 +3370,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
+      <c r="A6" s="83"/>
       <c r="B6" s="2" t="s">
         <v>50</v>
       </c>
@@ -3394,10 +3434,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="86" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="87" t="s">
         <v>55</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -3405,14 +3445,14 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="52"/>
-      <c r="B3" s="58"/>
+      <c r="A3" s="82"/>
+      <c r="B3" s="88"/>
       <c r="C3" s="8" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="53"/>
+      <c r="A4" s="83"/>
       <c r="B4" s="2" t="s">
         <v>56</v>
       </c>

</xml_diff>